<commit_message>
Update OFL, FONTLOG, Test document.
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="1898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1954">
   <si>
     <t>USV</t>
   </si>
@@ -5742,6 +5742,174 @@
   </si>
   <si>
     <t>uni00A0</t>
+  </si>
+  <si>
+    <t>1E7E0</t>
+  </si>
+  <si>
+    <t>u1E7E0</t>
+  </si>
+  <si>
+    <t>1E7E1</t>
+  </si>
+  <si>
+    <t>u1E7E1</t>
+  </si>
+  <si>
+    <t>1E7E2</t>
+  </si>
+  <si>
+    <t>u1E7E2</t>
+  </si>
+  <si>
+    <t>1E7E3</t>
+  </si>
+  <si>
+    <t>u1E7E3</t>
+  </si>
+  <si>
+    <t>1E7E4</t>
+  </si>
+  <si>
+    <t>u1E7E4</t>
+  </si>
+  <si>
+    <t>1E7E5</t>
+  </si>
+  <si>
+    <t>u1E7E5</t>
+  </si>
+  <si>
+    <t>1E7E6</t>
+  </si>
+  <si>
+    <t>u1E7E6</t>
+  </si>
+  <si>
+    <t>1E7E8</t>
+  </si>
+  <si>
+    <t>u1E7E8</t>
+  </si>
+  <si>
+    <t>1E7E9</t>
+  </si>
+  <si>
+    <t>u1E7E9</t>
+  </si>
+  <si>
+    <t>1E7EA</t>
+  </si>
+  <si>
+    <t>u1E7EA</t>
+  </si>
+  <si>
+    <t>1E7EB</t>
+  </si>
+  <si>
+    <t>u1E7EB</t>
+  </si>
+  <si>
+    <t>1E7ED</t>
+  </si>
+  <si>
+    <t>u1E7ED</t>
+  </si>
+  <si>
+    <t>1E7EE</t>
+  </si>
+  <si>
+    <t>u1E7EE</t>
+  </si>
+  <si>
+    <t>1E7F0</t>
+  </si>
+  <si>
+    <t>u1E7F0</t>
+  </si>
+  <si>
+    <t>1E7F1</t>
+  </si>
+  <si>
+    <t>u1E7F1</t>
+  </si>
+  <si>
+    <t>1E7F2</t>
+  </si>
+  <si>
+    <t>u1E7F2</t>
+  </si>
+  <si>
+    <t>1E7F3</t>
+  </si>
+  <si>
+    <t>u1E7F3</t>
+  </si>
+  <si>
+    <t>1E7F4</t>
+  </si>
+  <si>
+    <t>u1E7F4</t>
+  </si>
+  <si>
+    <t>1E7F5</t>
+  </si>
+  <si>
+    <t>u1E7F5</t>
+  </si>
+  <si>
+    <t>1E7F6</t>
+  </si>
+  <si>
+    <t>u1E7F6</t>
+  </si>
+  <si>
+    <t>1E7F7</t>
+  </si>
+  <si>
+    <t>u1E7F7</t>
+  </si>
+  <si>
+    <t>1E7F8</t>
+  </si>
+  <si>
+    <t>u1E7F8</t>
+  </si>
+  <si>
+    <t>1E7F9</t>
+  </si>
+  <si>
+    <t>u1E7F9</t>
+  </si>
+  <si>
+    <t>1E7FA</t>
+  </si>
+  <si>
+    <t>u1E7FA</t>
+  </si>
+  <si>
+    <t>1E7FB</t>
+  </si>
+  <si>
+    <t>u1E7FB</t>
+  </si>
+  <si>
+    <t>1E7FC</t>
+  </si>
+  <si>
+    <t>u1E7FC</t>
+  </si>
+  <si>
+    <t>1E7FD</t>
+  </si>
+  <si>
+    <t>u1E7FD</t>
+  </si>
+  <si>
+    <t>1E7FE</t>
+  </si>
+  <si>
+    <t>u1E7FE</t>
   </si>
 </sst>
 </file>
@@ -6067,10 +6235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1030"/>
+  <dimension ref="A1:I1058"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A1036" workbookViewId="0">
+      <selection activeCell="D1038" sqref="D1038"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18583,7 +18751,7 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="1025" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1025" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1025" t="s">
         <v>1798</v>
       </c>
@@ -18591,7 +18759,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="1026" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1026" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1026" t="s">
         <v>1799</v>
       </c>
@@ -18599,7 +18767,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="1027" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1027" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1027" t="s">
         <v>1800</v>
       </c>
@@ -18607,7 +18775,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="1028" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1028" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1028" t="s">
         <v>1801</v>
       </c>
@@ -18615,7 +18783,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="1029" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1029" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1029" t="s">
         <v>1802</v>
       </c>
@@ -18623,13 +18791,349 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="1030" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1030" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1030" t="s">
         <v>1803</v>
       </c>
       <c r="C1030">
         <v>2079</v>
       </c>
+    </row>
+    <row r="1031" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1031" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C1031">
+        <v>3001</v>
+      </c>
+      <c r="H1031"/>
+    </row>
+    <row r="1032" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1032" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C1032">
+        <v>3002</v>
+      </c>
+      <c r="H1032"/>
+    </row>
+    <row r="1033" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1033" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C1033">
+        <v>3003</v>
+      </c>
+      <c r="H1033"/>
+    </row>
+    <row r="1034" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1034" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C1034">
+        <v>3004</v>
+      </c>
+      <c r="H1034"/>
+    </row>
+    <row r="1035" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1035" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C1035">
+        <v>3005</v>
+      </c>
+      <c r="H1035"/>
+    </row>
+    <row r="1036" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1036" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C1036">
+        <v>3006</v>
+      </c>
+      <c r="H1036"/>
+    </row>
+    <row r="1037" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1037" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>1911</v>
+      </c>
+      <c r="C1037">
+        <v>3007</v>
+      </c>
+      <c r="H1037"/>
+    </row>
+    <row r="1038" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1038" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C1038">
+        <v>3008</v>
+      </c>
+      <c r="H1038"/>
+    </row>
+    <row r="1039" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1039" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C1039">
+        <v>3009</v>
+      </c>
+      <c r="H1039"/>
+    </row>
+    <row r="1040" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1040" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C1040">
+        <v>3010</v>
+      </c>
+      <c r="H1040"/>
+    </row>
+    <row r="1041" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1041" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>1919</v>
+      </c>
+      <c r="C1041">
+        <v>3011</v>
+      </c>
+      <c r="H1041"/>
+    </row>
+    <row r="1042" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1042" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C1042">
+        <v>3012</v>
+      </c>
+      <c r="H1042"/>
+    </row>
+    <row r="1043" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1043" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C1043">
+        <v>3013</v>
+      </c>
+      <c r="H1043"/>
+    </row>
+    <row r="1044" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1044" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>1925</v>
+      </c>
+      <c r="C1044">
+        <v>3014</v>
+      </c>
+      <c r="H1044"/>
+    </row>
+    <row r="1045" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1045" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C1045">
+        <v>3015</v>
+      </c>
+      <c r="H1045"/>
+    </row>
+    <row r="1046" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1046" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C1046">
+        <v>3016</v>
+      </c>
+      <c r="H1046"/>
+    </row>
+    <row r="1047" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1047" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C1047">
+        <v>3017</v>
+      </c>
+      <c r="H1047"/>
+    </row>
+    <row r="1048" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1048" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C1048">
+        <v>3018</v>
+      </c>
+      <c r="H1048"/>
+    </row>
+    <row r="1049" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1049" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C1049">
+        <v>3019</v>
+      </c>
+      <c r="H1049"/>
+    </row>
+    <row r="1050" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1050" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C1050">
+        <v>3020</v>
+      </c>
+      <c r="H1050"/>
+    </row>
+    <row r="1051" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1051" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C1051">
+        <v>3021</v>
+      </c>
+      <c r="H1051"/>
+    </row>
+    <row r="1052" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1052" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C1052">
+        <v>3022</v>
+      </c>
+      <c r="H1052"/>
+    </row>
+    <row r="1053" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1053" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C1053">
+        <v>3023</v>
+      </c>
+      <c r="H1053"/>
+    </row>
+    <row r="1054" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1054" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C1054">
+        <v>3024</v>
+      </c>
+      <c r="H1054"/>
+    </row>
+    <row r="1055" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1055" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C1055">
+        <v>3025</v>
+      </c>
+      <c r="H1055"/>
+    </row>
+    <row r="1056" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1056" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C1056">
+        <v>3026</v>
+      </c>
+      <c r="H1056"/>
+    </row>
+    <row r="1057" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C1057">
+        <v>3027</v>
+      </c>
+      <c r="H1057"/>
+    </row>
+    <row r="1058" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C1058">
+        <v>3028</v>
+      </c>
+      <c r="H1058"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1">

</xml_diff>

<commit_message>
Update glyph_data to include cv02. Add OpenType for cv02. Add test ftml.
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="1975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="1976">
   <si>
     <t>USV</t>
   </si>
@@ -5973,6 +5973,9 @@
   </si>
   <si>
     <t>DesignerOrder</t>
+  </si>
+  <si>
+    <t>cv02</t>
   </si>
 </sst>
 </file>
@@ -6300,7 +6303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1078"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A672" workbookViewId="0">
+      <selection activeCell="F682" sqref="F682"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16615,7 +16620,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="657" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
         <v>1158</v>
       </c>
@@ -16629,7 +16634,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="658" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
         <v>1160</v>
       </c>
@@ -16643,7 +16648,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="659" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
         <v>1162</v>
       </c>
@@ -16657,7 +16662,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="660" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
         <v>1164</v>
       </c>
@@ -16671,7 +16676,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="661" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
         <v>1166</v>
       </c>
@@ -16684,8 +16689,11 @@
       <c r="D661">
         <v>659</v>
       </c>
-    </row>
-    <row r="662" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G661" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="662" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
         <v>1168</v>
       </c>
@@ -16698,8 +16706,11 @@
       <c r="D662">
         <v>660</v>
       </c>
-    </row>
-    <row r="663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G662" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
         <v>1170</v>
       </c>
@@ -16712,8 +16723,11 @@
       <c r="D663">
         <v>661</v>
       </c>
-    </row>
-    <row r="664" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G663" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
         <v>1172</v>
       </c>
@@ -16726,8 +16740,11 @@
       <c r="D664">
         <v>662</v>
       </c>
-    </row>
-    <row r="665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G664" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
         <v>1174</v>
       </c>
@@ -16740,8 +16757,11 @@
       <c r="D665">
         <v>663</v>
       </c>
-    </row>
-    <row r="666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G665" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
         <v>1176</v>
       </c>
@@ -16754,8 +16774,11 @@
       <c r="D666">
         <v>664</v>
       </c>
-    </row>
-    <row r="667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G666" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
         <v>1178</v>
       </c>
@@ -16768,8 +16791,11 @@
       <c r="D667">
         <v>665</v>
       </c>
-    </row>
-    <row r="668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G667" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
         <v>1180</v>
       </c>
@@ -16782,8 +16808,11 @@
       <c r="D668">
         <v>666</v>
       </c>
-    </row>
-    <row r="669" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G668" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
         <v>1182</v>
       </c>
@@ -16796,8 +16825,11 @@
       <c r="D669">
         <v>667</v>
       </c>
-    </row>
-    <row r="670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G669" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
         <v>1184</v>
       </c>
@@ -16810,8 +16842,11 @@
       <c r="D670">
         <v>668</v>
       </c>
-    </row>
-    <row r="671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G670" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
         <v>1186</v>
       </c>
@@ -16824,8 +16859,11 @@
       <c r="D671">
         <v>669</v>
       </c>
-    </row>
-    <row r="672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G671" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
         <v>1188</v>
       </c>
@@ -16838,8 +16876,11 @@
       <c r="D672">
         <v>670</v>
       </c>
-    </row>
-    <row r="673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G672" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
         <v>1190</v>
       </c>
@@ -16852,8 +16893,11 @@
       <c r="D673">
         <v>671</v>
       </c>
-    </row>
-    <row r="674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G673" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
         <v>1192</v>
       </c>
@@ -16866,8 +16910,11 @@
       <c r="D674">
         <v>672</v>
       </c>
-    </row>
-    <row r="675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G674" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
         <v>1194</v>
       </c>
@@ -16880,8 +16927,11 @@
       <c r="D675">
         <v>673</v>
       </c>
-    </row>
-    <row r="676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G675" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
         <v>1196</v>
       </c>
@@ -16894,8 +16944,11 @@
       <c r="D676">
         <v>674</v>
       </c>
-    </row>
-    <row r="677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G676" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
         <v>1198</v>
       </c>
@@ -16908,8 +16961,11 @@
       <c r="D677">
         <v>675</v>
       </c>
-    </row>
-    <row r="678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G677" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
         <v>1200</v>
       </c>
@@ -16922,8 +16978,11 @@
       <c r="D678">
         <v>676</v>
       </c>
-    </row>
-    <row r="679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G678" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
         <v>1202</v>
       </c>
@@ -16936,8 +16995,11 @@
       <c r="D679">
         <v>677</v>
       </c>
-    </row>
-    <row r="680" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G679" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
         <v>1204</v>
       </c>
@@ -16950,8 +17012,11 @@
       <c r="D680">
         <v>678</v>
       </c>
-    </row>
-    <row r="681" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G680" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>1953</v>
       </c>
@@ -16961,8 +17026,11 @@
       <c r="D681">
         <v>679</v>
       </c>
-    </row>
-    <row r="682" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G681" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
         <v>1954</v>
       </c>
@@ -16972,8 +17040,11 @@
       <c r="D682">
         <v>680</v>
       </c>
-    </row>
-    <row r="683" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G682" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>1955</v>
       </c>
@@ -16983,8 +17054,11 @@
       <c r="D683">
         <v>681</v>
       </c>
-    </row>
-    <row r="684" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G683" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
         <v>1956</v>
       </c>
@@ -16994,8 +17068,11 @@
       <c r="D684">
         <v>682</v>
       </c>
-    </row>
-    <row r="685" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G684" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="685" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
         <v>1957</v>
       </c>
@@ -17005,8 +17082,11 @@
       <c r="D685">
         <v>683</v>
       </c>
-    </row>
-    <row r="686" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G685" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="686" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
         <v>1958</v>
       </c>
@@ -17016,8 +17096,11 @@
       <c r="D686">
         <v>684</v>
       </c>
-    </row>
-    <row r="687" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G686" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
         <v>1959</v>
       </c>
@@ -17027,8 +17110,11 @@
       <c r="D687">
         <v>685</v>
       </c>
-    </row>
-    <row r="688" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G687" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
         <v>1960</v>
       </c>
@@ -17037,6 +17123,9 @@
       </c>
       <c r="D688">
         <v>686</v>
+      </c>
+      <c r="G688" t="s">
+        <v>1975</v>
       </c>
     </row>
     <row r="689" spans="1:9" x14ac:dyDescent="0.25">
@@ -17049,6 +17138,9 @@
       <c r="D689">
         <v>687</v>
       </c>
+      <c r="G689" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
@@ -17060,6 +17152,9 @@
       <c r="D690">
         <v>688</v>
       </c>
+      <c r="G690" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="691" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
@@ -17071,6 +17166,9 @@
       <c r="D691">
         <v>689</v>
       </c>
+      <c r="G691" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="692" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
@@ -17082,6 +17180,9 @@
       <c r="D692">
         <v>690</v>
       </c>
+      <c r="G692" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="693" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
@@ -17093,6 +17194,9 @@
       <c r="D693">
         <v>691</v>
       </c>
+      <c r="G693" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="694" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
@@ -17104,6 +17208,9 @@
       <c r="D694">
         <v>692</v>
       </c>
+      <c r="G694" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="695" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
@@ -17115,6 +17222,9 @@
       <c r="D695">
         <v>693</v>
       </c>
+      <c r="G695" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="696" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
@@ -17126,6 +17236,9 @@
       <c r="D696">
         <v>694</v>
       </c>
+      <c r="G696" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="697" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
@@ -17137,6 +17250,9 @@
       <c r="D697">
         <v>695</v>
       </c>
+      <c r="G697" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="698" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
@@ -17148,6 +17264,9 @@
       <c r="D698">
         <v>696</v>
       </c>
+      <c r="G698" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="699" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
@@ -17159,6 +17278,9 @@
       <c r="D699">
         <v>697</v>
       </c>
+      <c r="G699" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="700" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
@@ -17169,6 +17291,9 @@
       </c>
       <c r="D700">
         <v>698</v>
+      </c>
+      <c r="G700" t="s">
+        <v>1975</v>
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add glyphs and code needed to make the cv02 feature with connected lines above the Ethi digits. Currently, the bars are too long or too short in cases. After feedback on the height the length will be adjusted.
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -6224,13 +6224,13 @@
     <t>numeralnarrow</t>
   </si>
   <si>
-    <t>numeral.init</t>
-  </si>
-  <si>
-    <t>numeral.medi</t>
-  </si>
-  <si>
-    <t>numeral.fina</t>
+    <t>numeralinit</t>
+  </si>
+  <si>
+    <t>numeralmedi</t>
+  </si>
+  <si>
+    <t>numeralfina</t>
   </si>
 </sst>
 </file>
@@ -6558,8 +6558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1145" workbookViewId="0">
-      <selection activeCell="J1163" sqref="J1163"/>
+    <sheetView tabSelected="1" topLeftCell="A1122" workbookViewId="0">
+      <selection activeCell="B1136" sqref="B1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deleted unnecessary .isol glyphs and just used a different class name in main.gdl
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">glyph_data!$A$1:$J$1</definedName>
-    <definedName name="glyph_data" localSheetId="0">glyph_data!$A$1:$J$1043</definedName>
+    <definedName name="glyph_data" localSheetId="0">glyph_data!$A$1:$J$1023</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3475" uniqueCount="1964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="1944">
   <si>
     <t>USV</t>
   </si>
@@ -5682,66 +5682,6 @@
   </si>
   <si>
     <t>cv02</t>
-  </si>
-  <si>
-    <t>uni1369.isol</t>
-  </si>
-  <si>
-    <t>uni136A.isol</t>
-  </si>
-  <si>
-    <t>uni136B.isol</t>
-  </si>
-  <si>
-    <t>uni136C.isol</t>
-  </si>
-  <si>
-    <t>uni136D.isol</t>
-  </si>
-  <si>
-    <t>uni136E.isol</t>
-  </si>
-  <si>
-    <t>uni136F.isol</t>
-  </si>
-  <si>
-    <t>uni1370.isol</t>
-  </si>
-  <si>
-    <t>uni1371.isol</t>
-  </si>
-  <si>
-    <t>uni1372.isol</t>
-  </si>
-  <si>
-    <t>uni1373.isol</t>
-  </si>
-  <si>
-    <t>uni1374.isol</t>
-  </si>
-  <si>
-    <t>uni1375.isol</t>
-  </si>
-  <si>
-    <t>uni1376.isol</t>
-  </si>
-  <si>
-    <t>uni1377.isol</t>
-  </si>
-  <si>
-    <t>uni1378.isol</t>
-  </si>
-  <si>
-    <t>uni1379.isol</t>
-  </si>
-  <si>
-    <t>uni137A.isol</t>
-  </si>
-  <si>
-    <t>uni137B.isol</t>
-  </si>
-  <si>
-    <t>uni137C.isol</t>
   </si>
   <si>
     <t>uni1369.init</t>
@@ -6265,10 +6205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1076"/>
+  <dimension ref="A1:J1056"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A663" workbookViewId="0">
-      <selection activeCell="A682" sqref="A682:XFD682"/>
+    <sheetView tabSelected="1" topLeftCell="A933" workbookViewId="0">
+      <selection activeCell="A951" sqref="A951"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15909,7 +15849,7 @@
         <v>1</v>
       </c>
       <c r="I611" s="1" t="s">
-        <v>1963</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="612" spans="1:9" x14ac:dyDescent="0.25">
@@ -20953,7 +20893,7 @@
         <v>1878</v>
       </c>
       <c r="D940">
-        <v>1020</v>
+        <v>1040</v>
       </c>
       <c r="G940" t="s">
         <v>1877</v>
@@ -20967,7 +20907,7 @@
         <v>1879</v>
       </c>
       <c r="D941">
-        <v>1021</v>
+        <v>1041</v>
       </c>
       <c r="G941" t="s">
         <v>1877</v>
@@ -20981,7 +20921,7 @@
         <v>1880</v>
       </c>
       <c r="D942">
-        <v>1022</v>
+        <v>1042</v>
       </c>
       <c r="G942" t="s">
         <v>1877</v>
@@ -20995,7 +20935,7 @@
         <v>1881</v>
       </c>
       <c r="D943">
-        <v>1023</v>
+        <v>1043</v>
       </c>
       <c r="G943" t="s">
         <v>1877</v>
@@ -21009,7 +20949,7 @@
         <v>1882</v>
       </c>
       <c r="D944">
-        <v>1024</v>
+        <v>1044</v>
       </c>
       <c r="G944" t="s">
         <v>1877</v>
@@ -21023,7 +20963,7 @@
         <v>1883</v>
       </c>
       <c r="D945">
-        <v>1025</v>
+        <v>1045</v>
       </c>
       <c r="G945" t="s">
         <v>1877</v>
@@ -21037,7 +20977,7 @@
         <v>1884</v>
       </c>
       <c r="D946">
-        <v>1026</v>
+        <v>1046</v>
       </c>
       <c r="G946" t="s">
         <v>1877</v>
@@ -21051,7 +20991,7 @@
         <v>1885</v>
       </c>
       <c r="D947">
-        <v>1027</v>
+        <v>1047</v>
       </c>
       <c r="G947" t="s">
         <v>1877</v>
@@ -21065,7 +21005,7 @@
         <v>1886</v>
       </c>
       <c r="D948">
-        <v>1028</v>
+        <v>1048</v>
       </c>
       <c r="G948" t="s">
         <v>1877</v>
@@ -21079,7 +21019,7 @@
         <v>1887</v>
       </c>
       <c r="D949">
-        <v>1029</v>
+        <v>1049</v>
       </c>
       <c r="G949" t="s">
         <v>1877</v>
@@ -21093,7 +21033,7 @@
         <v>1888</v>
       </c>
       <c r="D950">
-        <v>1030</v>
+        <v>1050</v>
       </c>
       <c r="G950" t="s">
         <v>1877</v>
@@ -21107,7 +21047,7 @@
         <v>1889</v>
       </c>
       <c r="D951">
-        <v>1031</v>
+        <v>1051</v>
       </c>
       <c r="G951" t="s">
         <v>1877</v>
@@ -21121,7 +21061,7 @@
         <v>1890</v>
       </c>
       <c r="D952">
-        <v>1032</v>
+        <v>1052</v>
       </c>
       <c r="G952" t="s">
         <v>1877</v>
@@ -21135,7 +21075,7 @@
         <v>1891</v>
       </c>
       <c r="D953">
-        <v>1033</v>
+        <v>1053</v>
       </c>
       <c r="G953" t="s">
         <v>1877</v>
@@ -21149,7 +21089,7 @@
         <v>1892</v>
       </c>
       <c r="D954">
-        <v>1034</v>
+        <v>1054</v>
       </c>
       <c r="G954" t="s">
         <v>1877</v>
@@ -21163,7 +21103,7 @@
         <v>1893</v>
       </c>
       <c r="D955">
-        <v>1035</v>
+        <v>1055</v>
       </c>
       <c r="G955" t="s">
         <v>1877</v>
@@ -21177,7 +21117,7 @@
         <v>1894</v>
       </c>
       <c r="D956">
-        <v>1036</v>
+        <v>1056</v>
       </c>
       <c r="G956" t="s">
         <v>1877</v>
@@ -21191,7 +21131,7 @@
         <v>1895</v>
       </c>
       <c r="D957">
-        <v>1037</v>
+        <v>1057</v>
       </c>
       <c r="G957" t="s">
         <v>1877</v>
@@ -21205,7 +21145,7 @@
         <v>1896</v>
       </c>
       <c r="D958">
-        <v>1038</v>
+        <v>1058</v>
       </c>
       <c r="G958" t="s">
         <v>1877</v>
@@ -21219,7 +21159,7 @@
         <v>1897</v>
       </c>
       <c r="D959">
-        <v>1039</v>
+        <v>1059</v>
       </c>
       <c r="G959" t="s">
         <v>1877</v>
@@ -21233,7 +21173,7 @@
         <v>1898</v>
       </c>
       <c r="D960">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="G960" t="s">
         <v>1877</v>
@@ -21247,7 +21187,7 @@
         <v>1899</v>
       </c>
       <c r="D961">
-        <v>1041</v>
+        <v>1061</v>
       </c>
       <c r="G961" t="s">
         <v>1877</v>
@@ -21261,7 +21201,7 @@
         <v>1900</v>
       </c>
       <c r="D962">
-        <v>1042</v>
+        <v>1062</v>
       </c>
       <c r="G962" t="s">
         <v>1877</v>
@@ -21275,7 +21215,7 @@
         <v>1901</v>
       </c>
       <c r="D963">
-        <v>1043</v>
+        <v>1063</v>
       </c>
       <c r="G963" t="s">
         <v>1877</v>
@@ -21289,7 +21229,7 @@
         <v>1902</v>
       </c>
       <c r="D964">
-        <v>1044</v>
+        <v>1064</v>
       </c>
       <c r="G964" t="s">
         <v>1877</v>
@@ -21303,7 +21243,7 @@
         <v>1903</v>
       </c>
       <c r="D965">
-        <v>1045</v>
+        <v>1065</v>
       </c>
       <c r="G965" t="s">
         <v>1877</v>
@@ -21317,7 +21257,7 @@
         <v>1904</v>
       </c>
       <c r="D966">
-        <v>1046</v>
+        <v>1066</v>
       </c>
       <c r="G966" t="s">
         <v>1877</v>
@@ -21331,7 +21271,7 @@
         <v>1905</v>
       </c>
       <c r="D967">
-        <v>1047</v>
+        <v>1067</v>
       </c>
       <c r="G967" t="s">
         <v>1877</v>
@@ -21345,7 +21285,7 @@
         <v>1906</v>
       </c>
       <c r="D968">
-        <v>1048</v>
+        <v>1068</v>
       </c>
       <c r="G968" t="s">
         <v>1877</v>
@@ -21359,7 +21299,7 @@
         <v>1907</v>
       </c>
       <c r="D969">
-        <v>1049</v>
+        <v>1069</v>
       </c>
       <c r="G969" t="s">
         <v>1877</v>
@@ -21373,7 +21313,7 @@
         <v>1908</v>
       </c>
       <c r="D970">
-        <v>1050</v>
+        <v>1070</v>
       </c>
       <c r="G970" t="s">
         <v>1877</v>
@@ -21387,7 +21327,7 @@
         <v>1909</v>
       </c>
       <c r="D971">
-        <v>1051</v>
+        <v>1071</v>
       </c>
       <c r="G971" t="s">
         <v>1877</v>
@@ -21401,7 +21341,7 @@
         <v>1910</v>
       </c>
       <c r="D972">
-        <v>1052</v>
+        <v>1072</v>
       </c>
       <c r="G972" t="s">
         <v>1877</v>
@@ -21415,7 +21355,7 @@
         <v>1911</v>
       </c>
       <c r="D973">
-        <v>1053</v>
+        <v>1073</v>
       </c>
       <c r="G973" t="s">
         <v>1877</v>
@@ -21429,7 +21369,7 @@
         <v>1912</v>
       </c>
       <c r="D974">
-        <v>1054</v>
+        <v>1074</v>
       </c>
       <c r="G974" t="s">
         <v>1877</v>
@@ -21443,7 +21383,7 @@
         <v>1913</v>
       </c>
       <c r="D975">
-        <v>1055</v>
+        <v>1075</v>
       </c>
       <c r="G975" t="s">
         <v>1877</v>
@@ -21457,7 +21397,7 @@
         <v>1914</v>
       </c>
       <c r="D976">
-        <v>1056</v>
+        <v>1076</v>
       </c>
       <c r="G976" t="s">
         <v>1877</v>
@@ -21471,7 +21411,7 @@
         <v>1915</v>
       </c>
       <c r="D977">
-        <v>1057</v>
+        <v>1077</v>
       </c>
       <c r="G977" t="s">
         <v>1877</v>
@@ -21485,7 +21425,7 @@
         <v>1916</v>
       </c>
       <c r="D978">
-        <v>1058</v>
+        <v>1078</v>
       </c>
       <c r="G978" t="s">
         <v>1877</v>
@@ -21499,7 +21439,7 @@
         <v>1917</v>
       </c>
       <c r="D979">
-        <v>1059</v>
+        <v>1079</v>
       </c>
       <c r="G979" t="s">
         <v>1877</v>
@@ -21513,7 +21453,7 @@
         <v>1918</v>
       </c>
       <c r="D980">
-        <v>1060</v>
+        <v>1080</v>
       </c>
       <c r="G980" t="s">
         <v>1877</v>
@@ -21527,7 +21467,7 @@
         <v>1919</v>
       </c>
       <c r="D981">
-        <v>1061</v>
+        <v>1081</v>
       </c>
       <c r="G981" t="s">
         <v>1877</v>
@@ -21541,7 +21481,7 @@
         <v>1920</v>
       </c>
       <c r="D982">
-        <v>1062</v>
+        <v>1082</v>
       </c>
       <c r="G982" t="s">
         <v>1877</v>
@@ -21555,7 +21495,7 @@
         <v>1921</v>
       </c>
       <c r="D983">
-        <v>1063</v>
+        <v>1083</v>
       </c>
       <c r="G983" t="s">
         <v>1877</v>
@@ -21569,7 +21509,7 @@
         <v>1922</v>
       </c>
       <c r="D984">
-        <v>1064</v>
+        <v>1084</v>
       </c>
       <c r="G984" t="s">
         <v>1877</v>
@@ -21583,7 +21523,7 @@
         <v>1923</v>
       </c>
       <c r="D985">
-        <v>1065</v>
+        <v>1085</v>
       </c>
       <c r="G985" t="s">
         <v>1877</v>
@@ -21597,7 +21537,7 @@
         <v>1924</v>
       </c>
       <c r="D986">
-        <v>1066</v>
+        <v>1086</v>
       </c>
       <c r="G986" t="s">
         <v>1877</v>
@@ -21611,7 +21551,7 @@
         <v>1925</v>
       </c>
       <c r="D987">
-        <v>1067</v>
+        <v>1087</v>
       </c>
       <c r="G987" t="s">
         <v>1877</v>
@@ -21625,7 +21565,7 @@
         <v>1926</v>
       </c>
       <c r="D988">
-        <v>1068</v>
+        <v>1088</v>
       </c>
       <c r="G988" t="s">
         <v>1877</v>
@@ -21639,7 +21579,7 @@
         <v>1927</v>
       </c>
       <c r="D989">
-        <v>1069</v>
+        <v>1089</v>
       </c>
       <c r="G989" t="s">
         <v>1877</v>
@@ -21653,7 +21593,7 @@
         <v>1928</v>
       </c>
       <c r="D990">
-        <v>1070</v>
+        <v>1090</v>
       </c>
       <c r="G990" t="s">
         <v>1877</v>
@@ -21667,7 +21607,7 @@
         <v>1929</v>
       </c>
       <c r="D991">
-        <v>1071</v>
+        <v>1091</v>
       </c>
       <c r="G991" t="s">
         <v>1877</v>
@@ -21681,7 +21621,7 @@
         <v>1930</v>
       </c>
       <c r="D992">
-        <v>1072</v>
+        <v>1092</v>
       </c>
       <c r="G992" t="s">
         <v>1877</v>
@@ -21695,7 +21635,7 @@
         <v>1931</v>
       </c>
       <c r="D993">
-        <v>1073</v>
+        <v>1093</v>
       </c>
       <c r="G993" t="s">
         <v>1877</v>
@@ -21709,7 +21649,7 @@
         <v>1932</v>
       </c>
       <c r="D994">
-        <v>1074</v>
+        <v>1094</v>
       </c>
       <c r="G994" t="s">
         <v>1877</v>
@@ -21723,7 +21663,7 @@
         <v>1933</v>
       </c>
       <c r="D995">
-        <v>1075</v>
+        <v>1095</v>
       </c>
       <c r="G995" t="s">
         <v>1877</v>
@@ -21737,7 +21677,7 @@
         <v>1934</v>
       </c>
       <c r="D996">
-        <v>1076</v>
+        <v>1096</v>
       </c>
       <c r="G996" t="s">
         <v>1877</v>
@@ -21751,7 +21691,7 @@
         <v>1935</v>
       </c>
       <c r="D997">
-        <v>1077</v>
+        <v>1097</v>
       </c>
       <c r="G997" t="s">
         <v>1877</v>
@@ -21765,7 +21705,7 @@
         <v>1936</v>
       </c>
       <c r="D998">
-        <v>1078</v>
+        <v>1098</v>
       </c>
       <c r="G998" t="s">
         <v>1877</v>
@@ -21779,7 +21719,7 @@
         <v>1937</v>
       </c>
       <c r="D999">
-        <v>1079</v>
+        <v>1099</v>
       </c>
       <c r="G999" t="s">
         <v>1877</v>
@@ -21787,13 +21727,13 @@
     </row>
     <row r="1000" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1000" t="s">
-        <v>1938</v>
+        <v>1855</v>
       </c>
       <c r="B1000" t="s">
-        <v>1938</v>
+        <v>1855</v>
       </c>
       <c r="D1000">
-        <v>1080</v>
+        <v>1100</v>
       </c>
       <c r="G1000" t="s">
         <v>1877</v>
@@ -21801,13 +21741,13 @@
     </row>
     <row r="1001" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1001" t="s">
-        <v>1939</v>
+        <v>1856</v>
       </c>
       <c r="B1001" t="s">
-        <v>1939</v>
+        <v>1856</v>
       </c>
       <c r="D1001">
-        <v>1081</v>
+        <v>1101</v>
       </c>
       <c r="G1001" t="s">
         <v>1877</v>
@@ -21815,13 +21755,13 @@
     </row>
     <row r="1002" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1002" t="s">
-        <v>1940</v>
+        <v>1857</v>
       </c>
       <c r="B1002" t="s">
-        <v>1940</v>
+        <v>1857</v>
       </c>
       <c r="D1002">
-        <v>1082</v>
+        <v>1102</v>
       </c>
       <c r="G1002" t="s">
         <v>1877</v>
@@ -21829,13 +21769,13 @@
     </row>
     <row r="1003" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1003" t="s">
-        <v>1941</v>
+        <v>1858</v>
       </c>
       <c r="B1003" t="s">
-        <v>1941</v>
+        <v>1858</v>
       </c>
       <c r="D1003">
-        <v>1083</v>
+        <v>1103</v>
       </c>
       <c r="G1003" t="s">
         <v>1877</v>
@@ -21843,13 +21783,13 @@
     </row>
     <row r="1004" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1004" t="s">
-        <v>1942</v>
+        <v>1859</v>
       </c>
       <c r="B1004" t="s">
-        <v>1942</v>
+        <v>1859</v>
       </c>
       <c r="D1004">
-        <v>1084</v>
+        <v>1104</v>
       </c>
       <c r="G1004" t="s">
         <v>1877</v>
@@ -21857,13 +21797,13 @@
     </row>
     <row r="1005" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1005" t="s">
-        <v>1943</v>
+        <v>1860</v>
       </c>
       <c r="B1005" t="s">
-        <v>1943</v>
+        <v>1860</v>
       </c>
       <c r="D1005">
-        <v>1085</v>
+        <v>1105</v>
       </c>
       <c r="G1005" t="s">
         <v>1877</v>
@@ -21871,13 +21811,13 @@
     </row>
     <row r="1006" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1006" t="s">
-        <v>1944</v>
+        <v>1861</v>
       </c>
       <c r="B1006" t="s">
-        <v>1944</v>
+        <v>1861</v>
       </c>
       <c r="D1006">
-        <v>1086</v>
+        <v>1106</v>
       </c>
       <c r="G1006" t="s">
         <v>1877</v>
@@ -21885,13 +21825,13 @@
     </row>
     <row r="1007" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
-        <v>1945</v>
+        <v>1862</v>
       </c>
       <c r="B1007" t="s">
-        <v>1945</v>
+        <v>1862</v>
       </c>
       <c r="D1007">
-        <v>1087</v>
+        <v>1107</v>
       </c>
       <c r="G1007" t="s">
         <v>1877</v>
@@ -21899,13 +21839,13 @@
     </row>
     <row r="1008" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1008" t="s">
-        <v>1946</v>
+        <v>1863</v>
       </c>
       <c r="B1008" t="s">
-        <v>1946</v>
+        <v>1863</v>
       </c>
       <c r="D1008">
-        <v>1088</v>
+        <v>1108</v>
       </c>
       <c r="G1008" t="s">
         <v>1877</v>
@@ -21913,13 +21853,13 @@
     </row>
     <row r="1009" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
-        <v>1947</v>
+        <v>1864</v>
       </c>
       <c r="B1009" t="s">
-        <v>1947</v>
+        <v>1864</v>
       </c>
       <c r="D1009">
-        <v>1089</v>
+        <v>1109</v>
       </c>
       <c r="G1009" t="s">
         <v>1877</v>
@@ -21927,13 +21867,13 @@
     </row>
     <row r="1010" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
-        <v>1948</v>
+        <v>1865</v>
       </c>
       <c r="B1010" t="s">
-        <v>1948</v>
+        <v>1865</v>
       </c>
       <c r="D1010">
-        <v>1090</v>
+        <v>1110</v>
       </c>
       <c r="G1010" t="s">
         <v>1877</v>
@@ -21941,13 +21881,13 @@
     </row>
     <row r="1011" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1011" t="s">
-        <v>1949</v>
+        <v>1866</v>
       </c>
       <c r="B1011" t="s">
-        <v>1949</v>
+        <v>1866</v>
       </c>
       <c r="D1011">
-        <v>1091</v>
+        <v>1111</v>
       </c>
       <c r="G1011" t="s">
         <v>1877</v>
@@ -21955,13 +21895,13 @@
     </row>
     <row r="1012" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1012" t="s">
-        <v>1950</v>
+        <v>1867</v>
       </c>
       <c r="B1012" t="s">
-        <v>1950</v>
+        <v>1867</v>
       </c>
       <c r="D1012">
-        <v>1092</v>
+        <v>1112</v>
       </c>
       <c r="G1012" t="s">
         <v>1877</v>
@@ -21969,13 +21909,13 @@
     </row>
     <row r="1013" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1013" t="s">
-        <v>1951</v>
+        <v>1868</v>
       </c>
       <c r="B1013" t="s">
-        <v>1951</v>
+        <v>1868</v>
       </c>
       <c r="D1013">
-        <v>1093</v>
+        <v>1113</v>
       </c>
       <c r="G1013" t="s">
         <v>1877</v>
@@ -21983,13 +21923,13 @@
     </row>
     <row r="1014" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1014" t="s">
-        <v>1952</v>
+        <v>1869</v>
       </c>
       <c r="B1014" t="s">
-        <v>1952</v>
+        <v>1869</v>
       </c>
       <c r="D1014">
-        <v>1094</v>
+        <v>1114</v>
       </c>
       <c r="G1014" t="s">
         <v>1877</v>
@@ -21997,13 +21937,13 @@
     </row>
     <row r="1015" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1015" t="s">
-        <v>1953</v>
+        <v>1870</v>
       </c>
       <c r="B1015" t="s">
-        <v>1953</v>
+        <v>1870</v>
       </c>
       <c r="D1015">
-        <v>1095</v>
+        <v>1115</v>
       </c>
       <c r="G1015" t="s">
         <v>1877</v>
@@ -22011,13 +21951,13 @@
     </row>
     <row r="1016" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
-        <v>1954</v>
+        <v>1871</v>
       </c>
       <c r="B1016" t="s">
-        <v>1954</v>
+        <v>1871</v>
       </c>
       <c r="D1016">
-        <v>1096</v>
+        <v>1116</v>
       </c>
       <c r="G1016" t="s">
         <v>1877</v>
@@ -22025,13 +21965,13 @@
     </row>
     <row r="1017" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1017" t="s">
-        <v>1955</v>
+        <v>1872</v>
       </c>
       <c r="B1017" t="s">
-        <v>1955</v>
+        <v>1872</v>
       </c>
       <c r="D1017">
-        <v>1097</v>
+        <v>1117</v>
       </c>
       <c r="G1017" t="s">
         <v>1877</v>
@@ -22039,13 +21979,13 @@
     </row>
     <row r="1018" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1018" t="s">
-        <v>1956</v>
+        <v>1873</v>
       </c>
       <c r="B1018" t="s">
-        <v>1956</v>
+        <v>1873</v>
       </c>
       <c r="D1018">
-        <v>1098</v>
+        <v>1118</v>
       </c>
       <c r="G1018" t="s">
         <v>1877</v>
@@ -22053,13 +21993,13 @@
     </row>
     <row r="1019" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1019" t="s">
-        <v>1957</v>
+        <v>1874</v>
       </c>
       <c r="B1019" t="s">
-        <v>1957</v>
+        <v>1874</v>
       </c>
       <c r="D1019">
-        <v>1099</v>
+        <v>1119</v>
       </c>
       <c r="G1019" t="s">
         <v>1877</v>
@@ -22067,802 +22007,522 @@
     </row>
     <row r="1020" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
-        <v>1855</v>
+        <v>1701</v>
       </c>
       <c r="B1020" t="s">
-        <v>1855</v>
+        <v>1701</v>
       </c>
       <c r="D1020">
-        <v>1100</v>
-      </c>
-      <c r="G1020" t="s">
-        <v>1877</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="1021" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
-        <v>1856</v>
+        <v>1702</v>
       </c>
       <c r="B1021" t="s">
-        <v>1856</v>
+        <v>1702</v>
       </c>
       <c r="D1021">
-        <v>1101</v>
-      </c>
-      <c r="G1021" t="s">
-        <v>1877</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1022" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1022" t="s">
-        <v>1857</v>
+        <v>1703</v>
       </c>
       <c r="B1022" t="s">
-        <v>1857</v>
+        <v>1703</v>
       </c>
       <c r="D1022">
-        <v>1102</v>
-      </c>
-      <c r="G1022" t="s">
-        <v>1877</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1023" t="s">
-        <v>1858</v>
+        <v>1704</v>
       </c>
       <c r="B1023" t="s">
-        <v>1858</v>
+        <v>1704</v>
       </c>
       <c r="D1023">
-        <v>1103</v>
-      </c>
-      <c r="G1023" t="s">
-        <v>1877</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1024" t="s">
-        <v>1859</v>
+        <v>1938</v>
       </c>
       <c r="B1024" t="s">
-        <v>1859</v>
+        <v>1938</v>
       </c>
       <c r="D1024">
-        <v>1104</v>
-      </c>
-      <c r="G1024" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1025" t="s">
-        <v>1860</v>
+        <v>1939</v>
       </c>
       <c r="B1025" t="s">
-        <v>1860</v>
+        <v>1939</v>
       </c>
       <c r="D1025">
-        <v>1105</v>
-      </c>
-      <c r="G1025" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1026" t="s">
-        <v>1861</v>
+        <v>1940</v>
       </c>
       <c r="B1026" t="s">
-        <v>1861</v>
+        <v>1940</v>
       </c>
       <c r="D1026">
-        <v>1106</v>
-      </c>
-      <c r="G1026" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
-        <v>1862</v>
+        <v>1941</v>
       </c>
       <c r="B1027" t="s">
-        <v>1862</v>
+        <v>1941</v>
       </c>
       <c r="D1027">
-        <v>1107</v>
-      </c>
-      <c r="G1027" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
-        <v>1863</v>
+        <v>1942</v>
       </c>
       <c r="B1028" t="s">
-        <v>1863</v>
+        <v>1942</v>
       </c>
       <c r="D1028">
-        <v>1108</v>
-      </c>
-      <c r="G1028" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1029" t="s">
-        <v>1864</v>
+        <v>1800</v>
       </c>
       <c r="B1029" t="s">
-        <v>1864</v>
+        <v>1800</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>1799</v>
       </c>
       <c r="D1029">
-        <v>1109</v>
-      </c>
-      <c r="G1029" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3001</v>
+      </c>
+      <c r="I1029"/>
+    </row>
+    <row r="1030" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1030" t="s">
-        <v>1865</v>
+        <v>1802</v>
       </c>
       <c r="B1030" t="s">
-        <v>1865</v>
+        <v>1802</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>1801</v>
       </c>
       <c r="D1030">
-        <v>1110</v>
-      </c>
-      <c r="G1030" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3002</v>
+      </c>
+      <c r="I1030"/>
+    </row>
+    <row r="1031" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1031" t="s">
-        <v>1866</v>
+        <v>1804</v>
       </c>
       <c r="B1031" t="s">
-        <v>1866</v>
+        <v>1804</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>1803</v>
       </c>
       <c r="D1031">
-        <v>1111</v>
-      </c>
-      <c r="G1031" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3003</v>
+      </c>
+      <c r="I1031"/>
+    </row>
+    <row r="1032" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1032" t="s">
-        <v>1867</v>
+        <v>1806</v>
       </c>
       <c r="B1032" t="s">
-        <v>1867</v>
+        <v>1806</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>1805</v>
       </c>
       <c r="D1032">
-        <v>1112</v>
-      </c>
-      <c r="G1032" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3004</v>
+      </c>
+      <c r="I1032"/>
+    </row>
+    <row r="1033" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1033" t="s">
-        <v>1868</v>
+        <v>1808</v>
       </c>
       <c r="B1033" t="s">
-        <v>1868</v>
+        <v>1808</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>1807</v>
       </c>
       <c r="D1033">
-        <v>1113</v>
-      </c>
-      <c r="G1033" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3005</v>
+      </c>
+      <c r="I1033"/>
+    </row>
+    <row r="1034" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
-        <v>1869</v>
+        <v>1810</v>
       </c>
       <c r="B1034" t="s">
-        <v>1869</v>
+        <v>1810</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>1809</v>
       </c>
       <c r="D1034">
-        <v>1114</v>
-      </c>
-      <c r="G1034" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3006</v>
+      </c>
+      <c r="I1034"/>
+    </row>
+    <row r="1035" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
-        <v>1870</v>
+        <v>1812</v>
       </c>
       <c r="B1035" t="s">
-        <v>1870</v>
+        <v>1812</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>1811</v>
       </c>
       <c r="D1035">
-        <v>1115</v>
-      </c>
-      <c r="G1035" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3007</v>
+      </c>
+      <c r="I1035"/>
+    </row>
+    <row r="1036" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1036" t="s">
-        <v>1871</v>
+        <v>1814</v>
       </c>
       <c r="B1036" t="s">
-        <v>1871</v>
+        <v>1814</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>1813</v>
       </c>
       <c r="D1036">
-        <v>1116</v>
-      </c>
-      <c r="G1036" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1037" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3008</v>
+      </c>
+      <c r="I1036"/>
+    </row>
+    <row r="1037" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
-        <v>1872</v>
+        <v>1816</v>
       </c>
       <c r="B1037" t="s">
-        <v>1872</v>
+        <v>1816</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>1815</v>
       </c>
       <c r="D1037">
-        <v>1117</v>
-      </c>
-      <c r="G1037" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1038" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3009</v>
+      </c>
+      <c r="I1037"/>
+    </row>
+    <row r="1038" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1038" t="s">
-        <v>1873</v>
+        <v>1818</v>
       </c>
       <c r="B1038" t="s">
-        <v>1873</v>
+        <v>1818</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>1817</v>
       </c>
       <c r="D1038">
-        <v>1118</v>
-      </c>
-      <c r="G1038" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3010</v>
+      </c>
+      <c r="I1038"/>
+    </row>
+    <row r="1039" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1039" t="s">
-        <v>1874</v>
+        <v>1820</v>
       </c>
       <c r="B1039" t="s">
-        <v>1874</v>
+        <v>1820</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>1819</v>
       </c>
       <c r="D1039">
-        <v>1119</v>
-      </c>
-      <c r="G1039" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3011</v>
+      </c>
+      <c r="I1039"/>
+    </row>
+    <row r="1040" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1040" t="s">
-        <v>1701</v>
+        <v>1822</v>
       </c>
       <c r="B1040" t="s">
-        <v>1701</v>
+        <v>1822</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>1821</v>
       </c>
       <c r="D1040">
-        <v>2007</v>
-      </c>
+        <v>3012</v>
+      </c>
+      <c r="I1040"/>
     </row>
     <row r="1041" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
-        <v>1702</v>
+        <v>1824</v>
       </c>
       <c r="B1041" t="s">
-        <v>1702</v>
+        <v>1824</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>1823</v>
       </c>
       <c r="D1041">
-        <v>2008</v>
-      </c>
+        <v>3013</v>
+      </c>
+      <c r="I1041"/>
     </row>
     <row r="1042" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1042" t="s">
-        <v>1703</v>
+        <v>1826</v>
       </c>
       <c r="B1042" t="s">
-        <v>1703</v>
+        <v>1826</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>1825</v>
       </c>
       <c r="D1042">
-        <v>2009</v>
-      </c>
+        <v>3014</v>
+      </c>
+      <c r="I1042"/>
     </row>
     <row r="1043" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1043" t="s">
-        <v>1704</v>
+        <v>1828</v>
       </c>
       <c r="B1043" t="s">
-        <v>1704</v>
+        <v>1828</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>1827</v>
       </c>
       <c r="D1043">
-        <v>2047</v>
-      </c>
+        <v>3015</v>
+      </c>
+      <c r="I1043"/>
     </row>
     <row r="1044" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1044" t="s">
-        <v>1958</v>
+        <v>1830</v>
       </c>
       <c r="B1044" t="s">
-        <v>1958</v>
+        <v>1830</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>1829</v>
       </c>
       <c r="D1044">
-        <v>2080</v>
-      </c>
+        <v>3016</v>
+      </c>
+      <c r="I1044"/>
     </row>
     <row r="1045" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1045" t="s">
-        <v>1959</v>
+        <v>1832</v>
       </c>
       <c r="B1045" t="s">
-        <v>1959</v>
+        <v>1832</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>1831</v>
       </c>
       <c r="D1045">
-        <v>2081</v>
-      </c>
+        <v>3017</v>
+      </c>
+      <c r="I1045"/>
     </row>
     <row r="1046" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1046" t="s">
-        <v>1960</v>
+        <v>1834</v>
       </c>
       <c r="B1046" t="s">
-        <v>1960</v>
+        <v>1834</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>1833</v>
       </c>
       <c r="D1046">
-        <v>2082</v>
-      </c>
+        <v>3018</v>
+      </c>
+      <c r="I1046"/>
     </row>
     <row r="1047" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1047" t="s">
-        <v>1961</v>
+        <v>1836</v>
       </c>
       <c r="B1047" t="s">
-        <v>1961</v>
+        <v>1836</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>1835</v>
       </c>
       <c r="D1047">
-        <v>2083</v>
-      </c>
+        <v>3019</v>
+      </c>
+      <c r="I1047"/>
     </row>
     <row r="1048" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1048" t="s">
-        <v>1962</v>
+        <v>1838</v>
       </c>
       <c r="B1048" t="s">
-        <v>1962</v>
+        <v>1838</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>1837</v>
       </c>
       <c r="D1048">
-        <v>2084</v>
-      </c>
+        <v>3020</v>
+      </c>
+      <c r="I1048"/>
     </row>
     <row r="1049" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1049" t="s">
-        <v>1800</v>
+        <v>1840</v>
       </c>
       <c r="B1049" t="s">
-        <v>1800</v>
+        <v>1840</v>
       </c>
       <c r="C1049" t="s">
-        <v>1799</v>
+        <v>1839</v>
       </c>
       <c r="D1049">
-        <v>3001</v>
+        <v>3021</v>
       </c>
       <c r="I1049"/>
     </row>
     <row r="1050" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1050" t="s">
-        <v>1802</v>
+        <v>1842</v>
       </c>
       <c r="B1050" t="s">
-        <v>1802</v>
+        <v>1842</v>
       </c>
       <c r="C1050" t="s">
-        <v>1801</v>
+        <v>1841</v>
       </c>
       <c r="D1050">
-        <v>3002</v>
+        <v>3022</v>
       </c>
       <c r="I1050"/>
     </row>
     <row r="1051" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
-        <v>1804</v>
+        <v>1844</v>
       </c>
       <c r="B1051" t="s">
-        <v>1804</v>
+        <v>1844</v>
       </c>
       <c r="C1051" t="s">
-        <v>1803</v>
+        <v>1843</v>
       </c>
       <c r="D1051">
-        <v>3003</v>
+        <v>3023</v>
       </c>
       <c r="I1051"/>
     </row>
     <row r="1052" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1052" t="s">
-        <v>1806</v>
+        <v>1846</v>
       </c>
       <c r="B1052" t="s">
-        <v>1806</v>
+        <v>1846</v>
       </c>
       <c r="C1052" t="s">
-        <v>1805</v>
+        <v>1845</v>
       </c>
       <c r="D1052">
-        <v>3004</v>
+        <v>3024</v>
       </c>
       <c r="I1052"/>
     </row>
     <row r="1053" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1053" t="s">
-        <v>1808</v>
+        <v>1848</v>
       </c>
       <c r="B1053" t="s">
-        <v>1808</v>
+        <v>1848</v>
       </c>
       <c r="C1053" t="s">
-        <v>1807</v>
+        <v>1847</v>
       </c>
       <c r="D1053">
-        <v>3005</v>
+        <v>3025</v>
       </c>
       <c r="I1053"/>
     </row>
     <row r="1054" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1054" t="s">
-        <v>1810</v>
+        <v>1850</v>
       </c>
       <c r="B1054" t="s">
-        <v>1810</v>
+        <v>1850</v>
       </c>
       <c r="C1054" t="s">
-        <v>1809</v>
+        <v>1849</v>
       </c>
       <c r="D1054">
-        <v>3006</v>
+        <v>3026</v>
       </c>
       <c r="I1054"/>
     </row>
     <row r="1055" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1055" t="s">
-        <v>1812</v>
+        <v>1852</v>
       </c>
       <c r="B1055" t="s">
-        <v>1812</v>
+        <v>1852</v>
       </c>
       <c r="C1055" t="s">
-        <v>1811</v>
+        <v>1851</v>
       </c>
       <c r="D1055">
-        <v>3007</v>
+        <v>3027</v>
       </c>
       <c r="I1055"/>
     </row>
     <row r="1056" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
-        <v>1814</v>
+        <v>1854</v>
       </c>
       <c r="B1056" t="s">
-        <v>1814</v>
+        <v>1854</v>
       </c>
       <c r="C1056" t="s">
-        <v>1813</v>
+        <v>1853</v>
       </c>
       <c r="D1056">
-        <v>3008</v>
+        <v>3028</v>
       </c>
       <c r="I1056"/>
-    </row>
-    <row r="1057" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1057" t="s">
-        <v>1816</v>
-      </c>
-      <c r="B1057" t="s">
-        <v>1816</v>
-      </c>
-      <c r="C1057" t="s">
-        <v>1815</v>
-      </c>
-      <c r="D1057">
-        <v>3009</v>
-      </c>
-      <c r="I1057"/>
-    </row>
-    <row r="1058" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1058" t="s">
-        <v>1818</v>
-      </c>
-      <c r="B1058" t="s">
-        <v>1818</v>
-      </c>
-      <c r="C1058" t="s">
-        <v>1817</v>
-      </c>
-      <c r="D1058">
-        <v>3010</v>
-      </c>
-      <c r="I1058"/>
-    </row>
-    <row r="1059" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1059" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B1059" t="s">
-        <v>1820</v>
-      </c>
-      <c r="C1059" t="s">
-        <v>1819</v>
-      </c>
-      <c r="D1059">
-        <v>3011</v>
-      </c>
-      <c r="I1059"/>
-    </row>
-    <row r="1060" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1060" t="s">
-        <v>1822</v>
-      </c>
-      <c r="B1060" t="s">
-        <v>1822</v>
-      </c>
-      <c r="C1060" t="s">
-        <v>1821</v>
-      </c>
-      <c r="D1060">
-        <v>3012</v>
-      </c>
-      <c r="I1060"/>
-    </row>
-    <row r="1061" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1061" t="s">
-        <v>1824</v>
-      </c>
-      <c r="B1061" t="s">
-        <v>1824</v>
-      </c>
-      <c r="C1061" t="s">
-        <v>1823</v>
-      </c>
-      <c r="D1061">
-        <v>3013</v>
-      </c>
-      <c r="I1061"/>
-    </row>
-    <row r="1062" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1062" t="s">
-        <v>1826</v>
-      </c>
-      <c r="B1062" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C1062" t="s">
-        <v>1825</v>
-      </c>
-      <c r="D1062">
-        <v>3014</v>
-      </c>
-      <c r="I1062"/>
-    </row>
-    <row r="1063" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1063" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B1063" t="s">
-        <v>1828</v>
-      </c>
-      <c r="C1063" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D1063">
-        <v>3015</v>
-      </c>
-      <c r="I1063"/>
-    </row>
-    <row r="1064" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1064" t="s">
-        <v>1830</v>
-      </c>
-      <c r="B1064" t="s">
-        <v>1830</v>
-      </c>
-      <c r="C1064" t="s">
-        <v>1829</v>
-      </c>
-      <c r="D1064">
-        <v>3016</v>
-      </c>
-      <c r="I1064"/>
-    </row>
-    <row r="1065" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1065" t="s">
-        <v>1832</v>
-      </c>
-      <c r="B1065" t="s">
-        <v>1832</v>
-      </c>
-      <c r="C1065" t="s">
-        <v>1831</v>
-      </c>
-      <c r="D1065">
-        <v>3017</v>
-      </c>
-      <c r="I1065"/>
-    </row>
-    <row r="1066" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1066" t="s">
-        <v>1834</v>
-      </c>
-      <c r="B1066" t="s">
-        <v>1834</v>
-      </c>
-      <c r="C1066" t="s">
-        <v>1833</v>
-      </c>
-      <c r="D1066">
-        <v>3018</v>
-      </c>
-      <c r="I1066"/>
-    </row>
-    <row r="1067" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1067" t="s">
-        <v>1836</v>
-      </c>
-      <c r="B1067" t="s">
-        <v>1836</v>
-      </c>
-      <c r="C1067" t="s">
-        <v>1835</v>
-      </c>
-      <c r="D1067">
-        <v>3019</v>
-      </c>
-      <c r="I1067"/>
-    </row>
-    <row r="1068" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1068" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B1068" t="s">
-        <v>1838</v>
-      </c>
-      <c r="C1068" t="s">
-        <v>1837</v>
-      </c>
-      <c r="D1068">
-        <v>3020</v>
-      </c>
-      <c r="I1068"/>
-    </row>
-    <row r="1069" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1069" t="s">
-        <v>1840</v>
-      </c>
-      <c r="B1069" t="s">
-        <v>1840</v>
-      </c>
-      <c r="C1069" t="s">
-        <v>1839</v>
-      </c>
-      <c r="D1069">
-        <v>3021</v>
-      </c>
-      <c r="I1069"/>
-    </row>
-    <row r="1070" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1070" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B1070" t="s">
-        <v>1842</v>
-      </c>
-      <c r="C1070" t="s">
-        <v>1841</v>
-      </c>
-      <c r="D1070">
-        <v>3022</v>
-      </c>
-      <c r="I1070"/>
-    </row>
-    <row r="1071" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1071" t="s">
-        <v>1844</v>
-      </c>
-      <c r="B1071" t="s">
-        <v>1844</v>
-      </c>
-      <c r="C1071" t="s">
-        <v>1843</v>
-      </c>
-      <c r="D1071">
-        <v>3023</v>
-      </c>
-      <c r="I1071"/>
-    </row>
-    <row r="1072" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1072" t="s">
-        <v>1846</v>
-      </c>
-      <c r="B1072" t="s">
-        <v>1846</v>
-      </c>
-      <c r="C1072" t="s">
-        <v>1845</v>
-      </c>
-      <c r="D1072">
-        <v>3024</v>
-      </c>
-      <c r="I1072"/>
-    </row>
-    <row r="1073" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1073" t="s">
-        <v>1848</v>
-      </c>
-      <c r="B1073" t="s">
-        <v>1848</v>
-      </c>
-      <c r="C1073" t="s">
-        <v>1847</v>
-      </c>
-      <c r="D1073">
-        <v>3025</v>
-      </c>
-      <c r="I1073"/>
-    </row>
-    <row r="1074" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1074" t="s">
-        <v>1850</v>
-      </c>
-      <c r="B1074" t="s">
-        <v>1850</v>
-      </c>
-      <c r="C1074" t="s">
-        <v>1849</v>
-      </c>
-      <c r="D1074">
-        <v>3026</v>
-      </c>
-      <c r="I1074"/>
-    </row>
-    <row r="1075" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1075" t="s">
-        <v>1852</v>
-      </c>
-      <c r="B1075" t="s">
-        <v>1852</v>
-      </c>
-      <c r="C1075" t="s">
-        <v>1851</v>
-      </c>
-      <c r="D1075">
-        <v>3027</v>
-      </c>
-      <c r="I1075"/>
-    </row>
-    <row r="1076" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1076" t="s">
-        <v>1854</v>
-      </c>
-      <c r="B1076" t="s">
-        <v>1854</v>
-      </c>
-      <c r="C1076" t="s">
-        <v>1853</v>
-      </c>
-      <c r="D1076">
-        <v>3028</v>
-      </c>
-      <c r="I1076"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">

</xml_diff>

<commit_message>
Added subscript and circle numbers to build.
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\evansl\repos\wstechfonts\font-abyssinica\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4BCCCF-922E-4095-A910-D7B5D503ED77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AED67-9C17-4D17-8E92-10D0086557B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23520" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">glyph_data!$A$1:$J$1</definedName>
-    <definedName name="glyph_data" localSheetId="0">glyph_data!$A$1:$J$1024</definedName>
+    <definedName name="glyph_data" localSheetId="0">glyph_data!$A$1:$J$1043</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="1946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="1983">
   <si>
     <t>USV</t>
   </si>
@@ -5887,6 +5887,117 @@
   </si>
   <si>
     <t>gzi.ligature</t>
+  </si>
+  <si>
+    <t>zero.inferior</t>
+  </si>
+  <si>
+    <t>one.inferior</t>
+  </si>
+  <si>
+    <t>two.inferior</t>
+  </si>
+  <si>
+    <t>three.inferior</t>
+  </si>
+  <si>
+    <t>four.inferior</t>
+  </si>
+  <si>
+    <t>five.inferior</t>
+  </si>
+  <si>
+    <t>six.inferior</t>
+  </si>
+  <si>
+    <t>seven.inferior</t>
+  </si>
+  <si>
+    <t>eight.inferior</t>
+  </si>
+  <si>
+    <t>nine.inferior</t>
+  </si>
+  <si>
+    <t>onecircle</t>
+  </si>
+  <si>
+    <t>twocircle</t>
+  </si>
+  <si>
+    <t>threecircle</t>
+  </si>
+  <si>
+    <t>fourcircle</t>
+  </si>
+  <si>
+    <t>fivecircle</t>
+  </si>
+  <si>
+    <t>sixcircle</t>
+  </si>
+  <si>
+    <t>sevencircle</t>
+  </si>
+  <si>
+    <t>eightcircle</t>
+  </si>
+  <si>
+    <t>ninecircle</t>
+  </si>
+  <si>
+    <t>uni2080</t>
+  </si>
+  <si>
+    <t>uni2081</t>
+  </si>
+  <si>
+    <t>uni2082</t>
+  </si>
+  <si>
+    <t>uni2083</t>
+  </si>
+  <si>
+    <t>uni2084</t>
+  </si>
+  <si>
+    <t>uni2085</t>
+  </si>
+  <si>
+    <t>uni2086</t>
+  </si>
+  <si>
+    <t>uni2087</t>
+  </si>
+  <si>
+    <t>uni2088</t>
+  </si>
+  <si>
+    <t>uni2460</t>
+  </si>
+  <si>
+    <t>uni2461</t>
+  </si>
+  <si>
+    <t>uni2462</t>
+  </si>
+  <si>
+    <t>uni2463</t>
+  </si>
+  <si>
+    <t>uni2464</t>
+  </si>
+  <si>
+    <t>uni2465</t>
+  </si>
+  <si>
+    <t>uni2466</t>
+  </si>
+  <si>
+    <t>uni2467</t>
+  </si>
+  <si>
+    <t>uni2468</t>
   </si>
 </sst>
 </file>
@@ -6212,10 +6323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1057"/>
+  <dimension ref="A1:J1076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A567" workbookViewId="0">
-      <selection activeCell="B552" sqref="B552"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19940,964 +20051,907 @@
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
-        <v>1616</v>
+        <v>1946</v>
       </c>
       <c r="B877" t="s">
-        <v>1616</v>
-      </c>
-      <c r="C877" s="2" t="s">
-        <v>1615</v>
+        <v>1965</v>
+      </c>
+      <c r="C877">
+        <v>2080</v>
       </c>
       <c r="D877">
-        <v>885</v>
-      </c>
-      <c r="G877" t="s">
-        <v>14</v>
-      </c>
-      <c r="H877">
-        <v>0</v>
+        <v>885.01</v>
       </c>
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
-        <v>1617</v>
+        <v>1947</v>
       </c>
       <c r="B878" t="s">
-        <v>1617</v>
+        <v>1966</v>
+      </c>
+      <c r="C878">
+        <v>2081</v>
       </c>
       <c r="D878">
-        <v>886</v>
-      </c>
-      <c r="G878" t="s">
-        <v>14</v>
-      </c>
-      <c r="H878">
-        <v>1</v>
-      </c>
-      <c r="I878" s="1" t="s">
-        <v>1615</v>
+        <v>885.02</v>
       </c>
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
-        <v>1619</v>
+        <v>1948</v>
       </c>
       <c r="B879" t="s">
-        <v>1619</v>
-      </c>
-      <c r="C879" s="2" t="s">
-        <v>1618</v>
+        <v>1967</v>
+      </c>
+      <c r="C879">
+        <v>2082</v>
       </c>
       <c r="D879">
-        <v>887</v>
+        <v>885.03</v>
       </c>
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C880">
+        <v>2083</v>
+      </c>
+      <c r="D880">
+        <v>885.04</v>
+      </c>
+    </row>
+    <row r="881" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C881">
+        <v>2084</v>
+      </c>
+      <c r="D881">
+        <v>885.05</v>
+      </c>
+    </row>
+    <row r="882" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C882">
+        <v>2085</v>
+      </c>
+      <c r="D882">
+        <v>885.06</v>
+      </c>
+    </row>
+    <row r="883" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C883">
+        <v>2086</v>
+      </c>
+      <c r="D883">
+        <v>885.07</v>
+      </c>
+    </row>
+    <row r="884" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B884" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C884">
+        <v>2087</v>
+      </c>
+      <c r="D884">
+        <v>885.08</v>
+      </c>
+    </row>
+    <row r="885" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C885">
+        <v>2088</v>
+      </c>
+      <c r="D885">
+        <v>885.09</v>
+      </c>
+    </row>
+    <row r="886" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C886">
+        <v>2088</v>
+      </c>
+      <c r="D886">
+        <v>885.11</v>
+      </c>
+    </row>
+    <row r="887" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C887">
+        <v>2460</v>
+      </c>
+      <c r="D887">
+        <v>885.12</v>
+      </c>
+    </row>
+    <row r="888" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C888">
+        <v>2461</v>
+      </c>
+      <c r="D888">
+        <v>885.13</v>
+      </c>
+    </row>
+    <row r="889" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C889">
+        <v>2462</v>
+      </c>
+      <c r="D889">
+        <v>885.14</v>
+      </c>
+    </row>
+    <row r="890" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C890">
+        <v>2463</v>
+      </c>
+      <c r="D890">
+        <v>885.15</v>
+      </c>
+    </row>
+    <row r="891" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C891">
+        <v>2464</v>
+      </c>
+      <c r="D891">
+        <v>885.16</v>
+      </c>
+    </row>
+    <row r="892" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C892">
+        <v>2465</v>
+      </c>
+      <c r="D892">
+        <v>885.17</v>
+      </c>
+    </row>
+    <row r="893" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C893">
+        <v>2466</v>
+      </c>
+      <c r="D893">
+        <v>885.18</v>
+      </c>
+    </row>
+    <row r="894" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C894">
+        <v>2467</v>
+      </c>
+      <c r="D894">
+        <v>885.19</v>
+      </c>
+    </row>
+    <row r="895" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C895">
+        <v>2468</v>
+      </c>
+      <c r="D895">
+        <v>885.21</v>
+      </c>
+    </row>
+    <row r="896" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C896" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D896">
+        <v>885</v>
+      </c>
+      <c r="G896" t="s">
+        <v>14</v>
+      </c>
+      <c r="H896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="897" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D897">
+        <v>886</v>
+      </c>
+      <c r="G897" t="s">
+        <v>14</v>
+      </c>
+      <c r="H897">
+        <v>1</v>
+      </c>
+      <c r="I897" s="1" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="898" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C898" s="2" t="s">
+        <v>1618</v>
+      </c>
+      <c r="D898">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="899" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
         <v>1621</v>
       </c>
-      <c r="B880" t="s">
+      <c r="B899" t="s">
         <v>1621</v>
       </c>
-      <c r="C880" s="2" t="s">
+      <c r="C899" s="2" t="s">
         <v>1620</v>
       </c>
-      <c r="D880">
+      <c r="D899">
         <v>888</v>
       </c>
     </row>
-    <row r="881" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A881" t="s">
+    <row r="900" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
         <v>1623</v>
       </c>
-      <c r="B881" t="s">
+      <c r="B900" t="s">
         <v>1623</v>
       </c>
-      <c r="C881" s="2" t="s">
+      <c r="C900" s="2" t="s">
         <v>1622</v>
       </c>
-      <c r="D881">
+      <c r="D900">
         <v>889</v>
       </c>
     </row>
-    <row r="882" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A882" t="s">
+    <row r="901" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
         <v>1625</v>
       </c>
-      <c r="B882" t="s">
+      <c r="B901" t="s">
         <v>1625</v>
       </c>
-      <c r="C882" s="2" t="s">
+      <c r="C901" s="2" t="s">
         <v>1624</v>
       </c>
-      <c r="D882">
+      <c r="D901">
         <v>890</v>
       </c>
     </row>
-    <row r="883" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A883" t="s">
+    <row r="902" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
         <v>1627</v>
       </c>
-      <c r="B883" t="s">
+      <c r="B902" t="s">
         <v>1627</v>
       </c>
-      <c r="C883" s="2" t="s">
+      <c r="C902" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="D883">
+      <c r="D902">
         <v>891</v>
       </c>
     </row>
-    <row r="884" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A884" t="s">
+    <row r="903" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
         <v>1629</v>
       </c>
-      <c r="B884" t="s">
+      <c r="B903" t="s">
         <v>1629</v>
       </c>
-      <c r="C884" s="2" t="s">
+      <c r="C903" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="D884">
+      <c r="D903">
         <v>892</v>
       </c>
     </row>
-    <row r="885" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A885" t="s">
+    <row r="904" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
         <v>1631</v>
       </c>
-      <c r="B885" t="s">
+      <c r="B904" t="s">
         <v>1631</v>
       </c>
-      <c r="C885" s="2" t="s">
+      <c r="C904" s="2" t="s">
         <v>1630</v>
       </c>
-      <c r="D885">
+      <c r="D904">
         <v>893</v>
       </c>
     </row>
-    <row r="886" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A886" t="s">
+    <row r="905" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
         <v>1633</v>
       </c>
-      <c r="B886" t="s">
+      <c r="B905" t="s">
         <v>1633</v>
       </c>
-      <c r="C886" s="2" t="s">
+      <c r="C905" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="D886">
+      <c r="D905">
         <v>894</v>
       </c>
     </row>
-    <row r="887" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A887" t="s">
+    <row r="906" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
         <v>1635</v>
       </c>
-      <c r="B887" t="s">
+      <c r="B906" t="s">
         <v>1635</v>
       </c>
-      <c r="C887" s="2" t="s">
+      <c r="C906" s="2" t="s">
         <v>1634</v>
       </c>
-      <c r="D887">
+      <c r="D906">
         <v>895</v>
       </c>
     </row>
-    <row r="888" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A888" t="s">
+    <row r="907" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
         <v>1637</v>
       </c>
-      <c r="B888" t="s">
+      <c r="B907" t="s">
         <v>1637</v>
       </c>
-      <c r="C888" s="2" t="s">
+      <c r="C907" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="D888">
+      <c r="D907">
         <v>896</v>
       </c>
     </row>
-    <row r="889" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A889" t="s">
+    <row r="908" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
         <v>1639</v>
       </c>
-      <c r="B889" t="s">
+      <c r="B908" t="s">
         <v>1639</v>
       </c>
-      <c r="C889" s="2" t="s">
+      <c r="C908" s="2" t="s">
         <v>1638</v>
       </c>
-      <c r="D889">
+      <c r="D908">
         <v>897</v>
       </c>
     </row>
-    <row r="890" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A890" t="s">
+    <row r="909" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
         <v>1641</v>
       </c>
-      <c r="B890" t="s">
+      <c r="B909" t="s">
         <v>1641</v>
       </c>
-      <c r="C890" s="2" t="s">
+      <c r="C909" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="D890">
+      <c r="D909">
         <v>898</v>
       </c>
     </row>
-    <row r="891" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A891" t="s">
+    <row r="910" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
         <v>1643</v>
       </c>
-      <c r="B891" t="s">
+      <c r="B910" t="s">
         <v>1643</v>
       </c>
-      <c r="C891" s="2" t="s">
+      <c r="C910" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="D891">
+      <c r="D910">
         <v>899</v>
       </c>
     </row>
-    <row r="892" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A892" t="s">
+    <row r="911" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
         <v>1647</v>
       </c>
-      <c r="B892" t="s">
+      <c r="B911" t="s">
         <v>1647</v>
       </c>
-      <c r="C892" s="2" t="s">
+      <c r="C911" s="2" t="s">
         <v>1646</v>
       </c>
-      <c r="D892">
+      <c r="D911">
         <v>900</v>
       </c>
     </row>
-    <row r="893" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A893" t="s">
+    <row r="912" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
         <v>1649</v>
       </c>
-      <c r="B893" t="s">
+      <c r="B912" t="s">
         <v>1649</v>
       </c>
-      <c r="C893" s="2" t="s">
+      <c r="C912" s="2" t="s">
         <v>1648</v>
       </c>
-      <c r="D893">
+      <c r="D912">
         <v>901</v>
       </c>
     </row>
-    <row r="894" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A894" t="s">
+    <row r="913" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
         <v>1651</v>
       </c>
-      <c r="B894" t="s">
+      <c r="B913" t="s">
         <v>1651</v>
       </c>
-      <c r="C894" s="2" t="s">
+      <c r="C913" s="2" t="s">
         <v>1650</v>
       </c>
-      <c r="D894">
+      <c r="D913">
         <v>902</v>
       </c>
     </row>
-    <row r="895" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A895" t="s">
+    <row r="914" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
         <v>1653</v>
       </c>
-      <c r="B895" t="s">
+      <c r="B914" t="s">
         <v>1653</v>
       </c>
-      <c r="C895" s="2" t="s">
+      <c r="C914" s="2" t="s">
         <v>1652</v>
       </c>
-      <c r="D895">
+      <c r="D914">
         <v>903</v>
       </c>
     </row>
-    <row r="896" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A896" t="s">
+    <row r="915" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A915" t="s">
         <v>1645</v>
       </c>
-      <c r="B896" t="s">
+      <c r="B915" t="s">
         <v>1645</v>
       </c>
-      <c r="C896" s="2" t="s">
+      <c r="C915" s="2" t="s">
         <v>1644</v>
       </c>
-      <c r="D896">
+      <c r="D915">
         <v>904</v>
       </c>
     </row>
-    <row r="897" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A897" t="s">
+    <row r="916" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A916" t="s">
         <v>1655</v>
       </c>
-      <c r="B897" t="s">
+      <c r="B916" t="s">
         <v>1655</v>
       </c>
-      <c r="C897" s="2" t="s">
+      <c r="C916" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="D897">
+      <c r="D916">
         <v>905</v>
       </c>
     </row>
-    <row r="898" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A898" t="s">
+    <row r="917" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
         <v>1657</v>
       </c>
-      <c r="B898" t="s">
+      <c r="B917" t="s">
         <v>1657</v>
       </c>
-      <c r="C898" s="2" t="s">
+      <c r="C917" s="2" t="s">
         <v>1656</v>
       </c>
-      <c r="D898">
+      <c r="D917">
         <v>906</v>
       </c>
     </row>
-    <row r="899" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A899" t="s">
+    <row r="918" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
         <v>1659</v>
       </c>
-      <c r="B899" t="s">
+      <c r="B918" t="s">
         <v>1659</v>
       </c>
-      <c r="C899" s="2" t="s">
+      <c r="C918" s="2" t="s">
         <v>1658</v>
       </c>
-      <c r="D899">
+      <c r="D918">
         <v>907</v>
       </c>
     </row>
-    <row r="900" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A900" t="s">
+    <row r="919" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A919" t="s">
         <v>1661</v>
       </c>
-      <c r="B900" t="s">
+      <c r="B919" t="s">
         <v>1661</v>
       </c>
-      <c r="C900" s="2" t="s">
+      <c r="C919" s="2" t="s">
         <v>1660</v>
       </c>
-      <c r="D900">
+      <c r="D919">
         <v>908</v>
       </c>
     </row>
-    <row r="901" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A901" t="s">
+    <row r="920" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A920" t="s">
         <v>1663</v>
       </c>
-      <c r="B901" t="s">
+      <c r="B920" t="s">
         <v>1663</v>
       </c>
-      <c r="C901" s="2" t="s">
+      <c r="C920" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="D901">
+      <c r="D920">
         <v>909</v>
       </c>
     </row>
-    <row r="902" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A902" t="s">
+    <row r="921" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A921" t="s">
         <v>1665</v>
       </c>
-      <c r="B902" t="s">
+      <c r="B921" t="s">
         <v>1665</v>
       </c>
-      <c r="C902" s="2" t="s">
+      <c r="C921" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="D902">
+      <c r="D921">
         <v>910</v>
       </c>
     </row>
-    <row r="903" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A903" t="s">
+    <row r="922" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A922" t="s">
         <v>1667</v>
       </c>
-      <c r="B903" t="s">
+      <c r="B922" t="s">
         <v>1667</v>
       </c>
-      <c r="C903" s="2" t="s">
+      <c r="C922" s="2" t="s">
         <v>1666</v>
       </c>
-      <c r="D903">
+      <c r="D922">
         <v>911</v>
       </c>
     </row>
-    <row r="904" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A904" t="s">
+    <row r="923" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A923" t="s">
         <v>1669</v>
       </c>
-      <c r="B904" t="s">
+      <c r="B923" t="s">
         <v>1669</v>
       </c>
-      <c r="C904" s="2" t="s">
+      <c r="C923" s="2" t="s">
         <v>1668</v>
       </c>
-      <c r="D904">
+      <c r="D923">
         <v>912</v>
       </c>
     </row>
-    <row r="905" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A905" t="s">
+    <row r="924" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A924" t="s">
         <v>1671</v>
       </c>
-      <c r="B905" t="s">
+      <c r="B924" t="s">
         <v>1671</v>
       </c>
-      <c r="C905" s="2" t="s">
+      <c r="C924" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="D905">
+      <c r="D924">
         <v>913</v>
       </c>
     </row>
-    <row r="906" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A906" t="s">
+    <row r="925" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
         <v>1673</v>
       </c>
-      <c r="B906" t="s">
+      <c r="B925" t="s">
         <v>1673</v>
       </c>
-      <c r="C906" s="2" t="s">
+      <c r="C925" s="2" t="s">
         <v>1672</v>
       </c>
-      <c r="D906">
+      <c r="D925">
         <v>914</v>
       </c>
     </row>
-    <row r="907" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A907" t="s">
+    <row r="926" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
         <v>1675</v>
       </c>
-      <c r="B907" t="s">
+      <c r="B926" t="s">
         <v>1675</v>
       </c>
-      <c r="C907" s="2" t="s">
+      <c r="C926" s="2" t="s">
         <v>1674</v>
       </c>
-      <c r="D907">
+      <c r="D926">
         <v>915</v>
       </c>
     </row>
-    <row r="908" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A908" t="s">
+    <row r="927" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
         <v>1677</v>
       </c>
-      <c r="B908" t="s">
+      <c r="B927" t="s">
         <v>1677</v>
       </c>
-      <c r="C908" s="2" t="s">
+      <c r="C927" s="2" t="s">
         <v>1676</v>
       </c>
-      <c r="D908">
+      <c r="D927">
         <v>916</v>
       </c>
     </row>
-    <row r="909" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A909" t="s">
+    <row r="928" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
         <v>1679</v>
       </c>
-      <c r="B909" t="s">
+      <c r="B928" t="s">
         <v>1679</v>
       </c>
-      <c r="C909" s="2" t="s">
+      <c r="C928" s="2" t="s">
         <v>1678</v>
       </c>
-      <c r="D909">
+      <c r="D928">
         <v>917</v>
-      </c>
-    </row>
-    <row r="910" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A910" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B910" t="s">
-        <v>1681</v>
-      </c>
-      <c r="C910" s="2" t="s">
-        <v>1680</v>
-      </c>
-      <c r="D910">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="911" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A911" t="s">
-        <v>1683</v>
-      </c>
-      <c r="B911" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C911" s="2" t="s">
-        <v>1682</v>
-      </c>
-      <c r="D911">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="912" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A912" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B912" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C912" s="2" t="s">
-        <v>1684</v>
-      </c>
-      <c r="D912">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="913" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A913" t="s">
-        <v>1687</v>
-      </c>
-      <c r="B913" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C913" s="2" t="s">
-        <v>1686</v>
-      </c>
-      <c r="D913">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="914" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A914" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B914" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C914" s="2" t="s">
-        <v>1688</v>
-      </c>
-      <c r="D914">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="915" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A915" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B915" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C915" s="2" t="s">
-        <v>1690</v>
-      </c>
-      <c r="D915">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="916" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A916" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B916" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C916" s="2" t="s">
-        <v>1692</v>
-      </c>
-      <c r="D916">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="917" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A917" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B917" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C917" s="2" t="s">
-        <v>1694</v>
-      </c>
-      <c r="D917">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="918" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A918" t="s">
-        <v>1697</v>
-      </c>
-      <c r="B918" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C918" s="2" t="s">
-        <v>1696</v>
-      </c>
-      <c r="D918">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="919" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A919" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B919" t="s">
-        <v>1699</v>
-      </c>
-      <c r="C919" s="2" t="s">
-        <v>1698</v>
-      </c>
-      <c r="D919">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="920" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A920" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B920" t="s">
-        <v>1700</v>
-      </c>
-      <c r="D920">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="921" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A921" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B921" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C921" s="2" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D921">
-        <v>1000</v>
-      </c>
-      <c r="G921" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="922" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A922" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B922" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C922" s="2" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D922">
-        <v>1001</v>
-      </c>
-      <c r="G922" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="923" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A923" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B923" t="s">
-        <v>1158</v>
-      </c>
-      <c r="C923" s="2" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D923">
-        <v>1002</v>
-      </c>
-      <c r="G923" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="924" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A924" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B924" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C924" s="2" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D924">
-        <v>1003</v>
-      </c>
-      <c r="G924" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="925" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A925" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B925" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C925" s="2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D925">
-        <v>1004</v>
-      </c>
-      <c r="G925" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="926" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A926" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B926" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C926" s="2" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D926">
-        <v>1005</v>
-      </c>
-      <c r="G926" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="927" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A927" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B927" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C927" s="2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D927">
-        <v>1006</v>
-      </c>
-      <c r="G927" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="928" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A928" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B928" t="s">
-        <v>1168</v>
-      </c>
-      <c r="C928" s="2" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D928">
-        <v>1007</v>
-      </c>
-      <c r="G928" t="s">
-        <v>1877</v>
       </c>
     </row>
     <row r="929" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A929" t="s">
-        <v>1170</v>
+        <v>1681</v>
       </c>
       <c r="B929" t="s">
-        <v>1170</v>
+        <v>1681</v>
       </c>
       <c r="C929" s="2" t="s">
-        <v>1169</v>
+        <v>1680</v>
       </c>
       <c r="D929">
-        <v>1008</v>
-      </c>
-      <c r="G929" t="s">
-        <v>1877</v>
+        <v>918</v>
       </c>
     </row>
     <row r="930" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A930" t="s">
-        <v>1172</v>
+        <v>1683</v>
       </c>
       <c r="B930" t="s">
-        <v>1172</v>
+        <v>1683</v>
       </c>
       <c r="C930" s="2" t="s">
-        <v>1171</v>
+        <v>1682</v>
       </c>
       <c r="D930">
-        <v>1009</v>
-      </c>
-      <c r="G930" t="s">
-        <v>1877</v>
+        <v>919</v>
       </c>
     </row>
     <row r="931" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A931" t="s">
-        <v>1174</v>
+        <v>1685</v>
       </c>
       <c r="B931" t="s">
-        <v>1174</v>
+        <v>1685</v>
       </c>
       <c r="C931" s="2" t="s">
-        <v>1173</v>
+        <v>1684</v>
       </c>
       <c r="D931">
-        <v>1010</v>
-      </c>
-      <c r="G931" t="s">
-        <v>1877</v>
+        <v>920</v>
       </c>
     </row>
     <row r="932" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A932" t="s">
-        <v>1176</v>
+        <v>1687</v>
       </c>
       <c r="B932" t="s">
-        <v>1176</v>
+        <v>1687</v>
       </c>
       <c r="C932" s="2" t="s">
-        <v>1175</v>
+        <v>1686</v>
       </c>
       <c r="D932">
-        <v>1011</v>
-      </c>
-      <c r="G932" t="s">
-        <v>1877</v>
+        <v>921</v>
       </c>
     </row>
     <row r="933" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A933" t="s">
-        <v>1178</v>
+        <v>1689</v>
       </c>
       <c r="B933" t="s">
-        <v>1178</v>
+        <v>1689</v>
       </c>
       <c r="C933" s="2" t="s">
-        <v>1177</v>
+        <v>1688</v>
       </c>
       <c r="D933">
-        <v>1012</v>
-      </c>
-      <c r="G933" t="s">
-        <v>1877</v>
+        <v>922</v>
       </c>
     </row>
     <row r="934" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A934" t="s">
-        <v>1180</v>
+        <v>1691</v>
       </c>
       <c r="B934" t="s">
-        <v>1180</v>
+        <v>1691</v>
       </c>
       <c r="C934" s="2" t="s">
-        <v>1179</v>
+        <v>1690</v>
       </c>
       <c r="D934">
-        <v>1013</v>
-      </c>
-      <c r="G934" t="s">
-        <v>1877</v>
+        <v>923</v>
       </c>
     </row>
     <row r="935" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A935" t="s">
-        <v>1182</v>
+        <v>1693</v>
       </c>
       <c r="B935" t="s">
-        <v>1182</v>
+        <v>1693</v>
       </c>
       <c r="C935" s="2" t="s">
-        <v>1181</v>
+        <v>1692</v>
       </c>
       <c r="D935">
-        <v>1014</v>
-      </c>
-      <c r="G935" t="s">
-        <v>1877</v>
+        <v>924</v>
       </c>
     </row>
     <row r="936" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A936" t="s">
-        <v>1184</v>
+        <v>1695</v>
       </c>
       <c r="B936" t="s">
-        <v>1184</v>
+        <v>1695</v>
       </c>
       <c r="C936" s="2" t="s">
-        <v>1183</v>
+        <v>1694</v>
       </c>
       <c r="D936">
-        <v>1015</v>
-      </c>
-      <c r="G936" t="s">
-        <v>1877</v>
+        <v>925</v>
       </c>
     </row>
     <row r="937" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A937" t="s">
-        <v>1186</v>
+        <v>1697</v>
       </c>
       <c r="B937" t="s">
-        <v>1186</v>
+        <v>1697</v>
       </c>
       <c r="C937" s="2" t="s">
-        <v>1185</v>
+        <v>1696</v>
       </c>
       <c r="D937">
-        <v>1016</v>
-      </c>
-      <c r="G937" t="s">
-        <v>1877</v>
+        <v>926</v>
       </c>
     </row>
     <row r="938" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A938" t="s">
-        <v>1188</v>
+        <v>1699</v>
       </c>
       <c r="B938" t="s">
-        <v>1188</v>
+        <v>1699</v>
       </c>
       <c r="C938" s="2" t="s">
-        <v>1187</v>
+        <v>1698</v>
       </c>
       <c r="D938">
-        <v>1017</v>
-      </c>
-      <c r="G938" t="s">
-        <v>1877</v>
+        <v>927</v>
       </c>
     </row>
     <row r="939" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A939" t="s">
-        <v>1190</v>
+        <v>1700</v>
       </c>
       <c r="B939" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C939" s="2" t="s">
-        <v>1189</v>
+        <v>1700</v>
       </c>
       <c r="D939">
-        <v>1018</v>
-      </c>
-      <c r="G939" t="s">
-        <v>1877</v>
+        <v>928</v>
       </c>
     </row>
     <row r="940" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A940" t="s">
-        <v>1192</v>
+        <v>1154</v>
       </c>
       <c r="B940" t="s">
-        <v>1192</v>
+        <v>1154</v>
       </c>
       <c r="C940" s="2" t="s">
-        <v>1191</v>
+        <v>1153</v>
       </c>
       <c r="D940">
-        <v>1019</v>
+        <v>1000</v>
       </c>
       <c r="G940" t="s">
         <v>1877</v>
@@ -20905,13 +20959,16 @@
     </row>
     <row r="941" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A941" t="s">
-        <v>1878</v>
+        <v>1156</v>
       </c>
       <c r="B941" t="s">
-        <v>1878</v>
+        <v>1156</v>
+      </c>
+      <c r="C941" s="2" t="s">
+        <v>1155</v>
       </c>
       <c r="D941">
-        <v>1040</v>
+        <v>1001</v>
       </c>
       <c r="G941" t="s">
         <v>1877</v>
@@ -20919,13 +20976,16 @@
     </row>
     <row r="942" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A942" t="s">
-        <v>1879</v>
+        <v>1158</v>
       </c>
       <c r="B942" t="s">
-        <v>1879</v>
+        <v>1158</v>
+      </c>
+      <c r="C942" s="2" t="s">
+        <v>1157</v>
       </c>
       <c r="D942">
-        <v>1041</v>
+        <v>1002</v>
       </c>
       <c r="G942" t="s">
         <v>1877</v>
@@ -20933,13 +20993,16 @@
     </row>
     <row r="943" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A943" t="s">
-        <v>1880</v>
+        <v>1160</v>
       </c>
       <c r="B943" t="s">
-        <v>1880</v>
+        <v>1160</v>
+      </c>
+      <c r="C943" s="2" t="s">
+        <v>1159</v>
       </c>
       <c r="D943">
-        <v>1042</v>
+        <v>1003</v>
       </c>
       <c r="G943" t="s">
         <v>1877</v>
@@ -20947,13 +21010,16 @@
     </row>
     <row r="944" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A944" t="s">
-        <v>1881</v>
+        <v>1162</v>
       </c>
       <c r="B944" t="s">
-        <v>1881</v>
+        <v>1162</v>
+      </c>
+      <c r="C944" s="2" t="s">
+        <v>1161</v>
       </c>
       <c r="D944">
-        <v>1043</v>
+        <v>1004</v>
       </c>
       <c r="G944" t="s">
         <v>1877</v>
@@ -20961,13 +21027,16 @@
     </row>
     <row r="945" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A945" t="s">
-        <v>1882</v>
+        <v>1164</v>
       </c>
       <c r="B945" t="s">
-        <v>1882</v>
+        <v>1164</v>
+      </c>
+      <c r="C945" s="2" t="s">
+        <v>1163</v>
       </c>
       <c r="D945">
-        <v>1044</v>
+        <v>1005</v>
       </c>
       <c r="G945" t="s">
         <v>1877</v>
@@ -20975,13 +21044,16 @@
     </row>
     <row r="946" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A946" t="s">
-        <v>1883</v>
+        <v>1166</v>
       </c>
       <c r="B946" t="s">
-        <v>1883</v>
+        <v>1166</v>
+      </c>
+      <c r="C946" s="2" t="s">
+        <v>1165</v>
       </c>
       <c r="D946">
-        <v>1045</v>
+        <v>1006</v>
       </c>
       <c r="G946" t="s">
         <v>1877</v>
@@ -20989,13 +21061,16 @@
     </row>
     <row r="947" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A947" t="s">
-        <v>1884</v>
+        <v>1168</v>
       </c>
       <c r="B947" t="s">
-        <v>1884</v>
+        <v>1168</v>
+      </c>
+      <c r="C947" s="2" t="s">
+        <v>1167</v>
       </c>
       <c r="D947">
-        <v>1046</v>
+        <v>1007</v>
       </c>
       <c r="G947" t="s">
         <v>1877</v>
@@ -21003,13 +21078,16 @@
     </row>
     <row r="948" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A948" t="s">
-        <v>1885</v>
+        <v>1170</v>
       </c>
       <c r="B948" t="s">
-        <v>1885</v>
+        <v>1170</v>
+      </c>
+      <c r="C948" s="2" t="s">
+        <v>1169</v>
       </c>
       <c r="D948">
-        <v>1047</v>
+        <v>1008</v>
       </c>
       <c r="G948" t="s">
         <v>1877</v>
@@ -21017,13 +21095,16 @@
     </row>
     <row r="949" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A949" t="s">
-        <v>1886</v>
+        <v>1172</v>
       </c>
       <c r="B949" t="s">
-        <v>1886</v>
+        <v>1172</v>
+      </c>
+      <c r="C949" s="2" t="s">
+        <v>1171</v>
       </c>
       <c r="D949">
-        <v>1048</v>
+        <v>1009</v>
       </c>
       <c r="G949" t="s">
         <v>1877</v>
@@ -21031,13 +21112,16 @@
     </row>
     <row r="950" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A950" t="s">
-        <v>1887</v>
+        <v>1174</v>
       </c>
       <c r="B950" t="s">
-        <v>1887</v>
+        <v>1174</v>
+      </c>
+      <c r="C950" s="2" t="s">
+        <v>1173</v>
       </c>
       <c r="D950">
-        <v>1049</v>
+        <v>1010</v>
       </c>
       <c r="G950" t="s">
         <v>1877</v>
@@ -21045,13 +21129,16 @@
     </row>
     <row r="951" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A951" t="s">
-        <v>1888</v>
+        <v>1176</v>
       </c>
       <c r="B951" t="s">
-        <v>1888</v>
+        <v>1176</v>
+      </c>
+      <c r="C951" s="2" t="s">
+        <v>1175</v>
       </c>
       <c r="D951">
-        <v>1050</v>
+        <v>1011</v>
       </c>
       <c r="G951" t="s">
         <v>1877</v>
@@ -21059,13 +21146,16 @@
     </row>
     <row r="952" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
-        <v>1889</v>
+        <v>1178</v>
       </c>
       <c r="B952" t="s">
-        <v>1889</v>
+        <v>1178</v>
+      </c>
+      <c r="C952" s="2" t="s">
+        <v>1177</v>
       </c>
       <c r="D952">
-        <v>1051</v>
+        <v>1012</v>
       </c>
       <c r="G952" t="s">
         <v>1877</v>
@@ -21073,13 +21163,16 @@
     </row>
     <row r="953" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A953" t="s">
-        <v>1890</v>
+        <v>1180</v>
       </c>
       <c r="B953" t="s">
-        <v>1890</v>
+        <v>1180</v>
+      </c>
+      <c r="C953" s="2" t="s">
+        <v>1179</v>
       </c>
       <c r="D953">
-        <v>1052</v>
+        <v>1013</v>
       </c>
       <c r="G953" t="s">
         <v>1877</v>
@@ -21087,13 +21180,16 @@
     </row>
     <row r="954" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A954" t="s">
-        <v>1891</v>
+        <v>1182</v>
       </c>
       <c r="B954" t="s">
-        <v>1891</v>
+        <v>1182</v>
+      </c>
+      <c r="C954" s="2" t="s">
+        <v>1181</v>
       </c>
       <c r="D954">
-        <v>1053</v>
+        <v>1014</v>
       </c>
       <c r="G954" t="s">
         <v>1877</v>
@@ -21101,13 +21197,16 @@
     </row>
     <row r="955" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A955" t="s">
-        <v>1892</v>
+        <v>1184</v>
       </c>
       <c r="B955" t="s">
-        <v>1892</v>
+        <v>1184</v>
+      </c>
+      <c r="C955" s="2" t="s">
+        <v>1183</v>
       </c>
       <c r="D955">
-        <v>1054</v>
+        <v>1015</v>
       </c>
       <c r="G955" t="s">
         <v>1877</v>
@@ -21115,13 +21214,16 @@
     </row>
     <row r="956" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A956" t="s">
-        <v>1893</v>
+        <v>1186</v>
       </c>
       <c r="B956" t="s">
-        <v>1893</v>
+        <v>1186</v>
+      </c>
+      <c r="C956" s="2" t="s">
+        <v>1185</v>
       </c>
       <c r="D956">
-        <v>1055</v>
+        <v>1016</v>
       </c>
       <c r="G956" t="s">
         <v>1877</v>
@@ -21129,13 +21231,16 @@
     </row>
     <row r="957" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A957" t="s">
-        <v>1894</v>
+        <v>1188</v>
       </c>
       <c r="B957" t="s">
-        <v>1894</v>
+        <v>1188</v>
+      </c>
+      <c r="C957" s="2" t="s">
+        <v>1187</v>
       </c>
       <c r="D957">
-        <v>1056</v>
+        <v>1017</v>
       </c>
       <c r="G957" t="s">
         <v>1877</v>
@@ -21143,13 +21248,16 @@
     </row>
     <row r="958" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A958" t="s">
-        <v>1895</v>
+        <v>1190</v>
       </c>
       <c r="B958" t="s">
-        <v>1895</v>
+        <v>1190</v>
+      </c>
+      <c r="C958" s="2" t="s">
+        <v>1189</v>
       </c>
       <c r="D958">
-        <v>1057</v>
+        <v>1018</v>
       </c>
       <c r="G958" t="s">
         <v>1877</v>
@@ -21157,13 +21265,16 @@
     </row>
     <row r="959" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A959" t="s">
-        <v>1896</v>
+        <v>1192</v>
       </c>
       <c r="B959" t="s">
-        <v>1896</v>
+        <v>1192</v>
+      </c>
+      <c r="C959" s="2" t="s">
+        <v>1191</v>
       </c>
       <c r="D959">
-        <v>1058</v>
+        <v>1019</v>
       </c>
       <c r="G959" t="s">
         <v>1877</v>
@@ -21171,13 +21282,13 @@
     </row>
     <row r="960" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A960" t="s">
-        <v>1897</v>
+        <v>1878</v>
       </c>
       <c r="B960" t="s">
-        <v>1897</v>
+        <v>1878</v>
       </c>
       <c r="D960">
-        <v>1059</v>
+        <v>1040</v>
       </c>
       <c r="G960" t="s">
         <v>1877</v>
@@ -21185,13 +21296,13 @@
     </row>
     <row r="961" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A961" t="s">
-        <v>1898</v>
+        <v>1879</v>
       </c>
       <c r="B961" t="s">
-        <v>1898</v>
+        <v>1879</v>
       </c>
       <c r="D961">
-        <v>1060</v>
+        <v>1041</v>
       </c>
       <c r="G961" t="s">
         <v>1877</v>
@@ -21199,13 +21310,13 @@
     </row>
     <row r="962" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A962" t="s">
-        <v>1899</v>
+        <v>1880</v>
       </c>
       <c r="B962" t="s">
-        <v>1899</v>
+        <v>1880</v>
       </c>
       <c r="D962">
-        <v>1061</v>
+        <v>1042</v>
       </c>
       <c r="G962" t="s">
         <v>1877</v>
@@ -21213,13 +21324,13 @@
     </row>
     <row r="963" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A963" t="s">
-        <v>1900</v>
+        <v>1881</v>
       </c>
       <c r="B963" t="s">
-        <v>1900</v>
+        <v>1881</v>
       </c>
       <c r="D963">
-        <v>1062</v>
+        <v>1043</v>
       </c>
       <c r="G963" t="s">
         <v>1877</v>
@@ -21227,13 +21338,13 @@
     </row>
     <row r="964" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A964" t="s">
-        <v>1901</v>
+        <v>1882</v>
       </c>
       <c r="B964" t="s">
-        <v>1901</v>
+        <v>1882</v>
       </c>
       <c r="D964">
-        <v>1063</v>
+        <v>1044</v>
       </c>
       <c r="G964" t="s">
         <v>1877</v>
@@ -21241,13 +21352,13 @@
     </row>
     <row r="965" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A965" t="s">
-        <v>1902</v>
+        <v>1883</v>
       </c>
       <c r="B965" t="s">
-        <v>1902</v>
+        <v>1883</v>
       </c>
       <c r="D965">
-        <v>1064</v>
+        <v>1045</v>
       </c>
       <c r="G965" t="s">
         <v>1877</v>
@@ -21255,13 +21366,13 @@
     </row>
     <row r="966" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A966" t="s">
-        <v>1903</v>
+        <v>1884</v>
       </c>
       <c r="B966" t="s">
-        <v>1903</v>
+        <v>1884</v>
       </c>
       <c r="D966">
-        <v>1065</v>
+        <v>1046</v>
       </c>
       <c r="G966" t="s">
         <v>1877</v>
@@ -21269,13 +21380,13 @@
     </row>
     <row r="967" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A967" t="s">
-        <v>1904</v>
+        <v>1885</v>
       </c>
       <c r="B967" t="s">
-        <v>1904</v>
+        <v>1885</v>
       </c>
       <c r="D967">
-        <v>1066</v>
+        <v>1047</v>
       </c>
       <c r="G967" t="s">
         <v>1877</v>
@@ -21283,13 +21394,13 @@
     </row>
     <row r="968" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A968" t="s">
-        <v>1905</v>
+        <v>1886</v>
       </c>
       <c r="B968" t="s">
-        <v>1905</v>
+        <v>1886</v>
       </c>
       <c r="D968">
-        <v>1067</v>
+        <v>1048</v>
       </c>
       <c r="G968" t="s">
         <v>1877</v>
@@ -21297,13 +21408,13 @@
     </row>
     <row r="969" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A969" t="s">
-        <v>1906</v>
+        <v>1887</v>
       </c>
       <c r="B969" t="s">
-        <v>1906</v>
+        <v>1887</v>
       </c>
       <c r="D969">
-        <v>1068</v>
+        <v>1049</v>
       </c>
       <c r="G969" t="s">
         <v>1877</v>
@@ -21311,13 +21422,13 @@
     </row>
     <row r="970" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A970" t="s">
-        <v>1907</v>
+        <v>1888</v>
       </c>
       <c r="B970" t="s">
-        <v>1907</v>
+        <v>1888</v>
       </c>
       <c r="D970">
-        <v>1069</v>
+        <v>1050</v>
       </c>
       <c r="G970" t="s">
         <v>1877</v>
@@ -21325,13 +21436,13 @@
     </row>
     <row r="971" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A971" t="s">
-        <v>1908</v>
+        <v>1889</v>
       </c>
       <c r="B971" t="s">
-        <v>1908</v>
+        <v>1889</v>
       </c>
       <c r="D971">
-        <v>1070</v>
+        <v>1051</v>
       </c>
       <c r="G971" t="s">
         <v>1877</v>
@@ -21339,13 +21450,13 @@
     </row>
     <row r="972" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A972" t="s">
-        <v>1909</v>
+        <v>1890</v>
       </c>
       <c r="B972" t="s">
-        <v>1909</v>
+        <v>1890</v>
       </c>
       <c r="D972">
-        <v>1071</v>
+        <v>1052</v>
       </c>
       <c r="G972" t="s">
         <v>1877</v>
@@ -21353,13 +21464,13 @@
     </row>
     <row r="973" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A973" t="s">
-        <v>1910</v>
+        <v>1891</v>
       </c>
       <c r="B973" t="s">
-        <v>1910</v>
+        <v>1891</v>
       </c>
       <c r="D973">
-        <v>1072</v>
+        <v>1053</v>
       </c>
       <c r="G973" t="s">
         <v>1877</v>
@@ -21367,13 +21478,13 @@
     </row>
     <row r="974" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A974" t="s">
-        <v>1911</v>
+        <v>1892</v>
       </c>
       <c r="B974" t="s">
-        <v>1911</v>
+        <v>1892</v>
       </c>
       <c r="D974">
-        <v>1073</v>
+        <v>1054</v>
       </c>
       <c r="G974" t="s">
         <v>1877</v>
@@ -21381,13 +21492,13 @@
     </row>
     <row r="975" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A975" t="s">
-        <v>1912</v>
+        <v>1893</v>
       </c>
       <c r="B975" t="s">
-        <v>1912</v>
+        <v>1893</v>
       </c>
       <c r="D975">
-        <v>1074</v>
+        <v>1055</v>
       </c>
       <c r="G975" t="s">
         <v>1877</v>
@@ -21395,13 +21506,13 @@
     </row>
     <row r="976" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A976" t="s">
-        <v>1913</v>
+        <v>1894</v>
       </c>
       <c r="B976" t="s">
-        <v>1913</v>
+        <v>1894</v>
       </c>
       <c r="D976">
-        <v>1075</v>
+        <v>1056</v>
       </c>
       <c r="G976" t="s">
         <v>1877</v>
@@ -21409,13 +21520,13 @@
     </row>
     <row r="977" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A977" t="s">
-        <v>1914</v>
+        <v>1895</v>
       </c>
       <c r="B977" t="s">
-        <v>1914</v>
+        <v>1895</v>
       </c>
       <c r="D977">
-        <v>1076</v>
+        <v>1057</v>
       </c>
       <c r="G977" t="s">
         <v>1877</v>
@@ -21423,13 +21534,13 @@
     </row>
     <row r="978" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A978" t="s">
-        <v>1915</v>
+        <v>1896</v>
       </c>
       <c r="B978" t="s">
-        <v>1915</v>
+        <v>1896</v>
       </c>
       <c r="D978">
-        <v>1077</v>
+        <v>1058</v>
       </c>
       <c r="G978" t="s">
         <v>1877</v>
@@ -21437,13 +21548,13 @@
     </row>
     <row r="979" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A979" t="s">
-        <v>1916</v>
+        <v>1897</v>
       </c>
       <c r="B979" t="s">
-        <v>1916</v>
+        <v>1897</v>
       </c>
       <c r="D979">
-        <v>1078</v>
+        <v>1059</v>
       </c>
       <c r="G979" t="s">
         <v>1877</v>
@@ -21451,13 +21562,13 @@
     </row>
     <row r="980" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A980" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
       <c r="B980" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
       <c r="D980">
-        <v>1079</v>
+        <v>1060</v>
       </c>
       <c r="G980" t="s">
         <v>1877</v>
@@ -21465,13 +21576,13 @@
     </row>
     <row r="981" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A981" t="s">
-        <v>1918</v>
+        <v>1899</v>
       </c>
       <c r="B981" t="s">
-        <v>1918</v>
+        <v>1899</v>
       </c>
       <c r="D981">
-        <v>1080</v>
+        <v>1061</v>
       </c>
       <c r="G981" t="s">
         <v>1877</v>
@@ -21479,13 +21590,13 @@
     </row>
     <row r="982" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A982" t="s">
-        <v>1919</v>
+        <v>1900</v>
       </c>
       <c r="B982" t="s">
-        <v>1919</v>
+        <v>1900</v>
       </c>
       <c r="D982">
-        <v>1081</v>
+        <v>1062</v>
       </c>
       <c r="G982" t="s">
         <v>1877</v>
@@ -21493,13 +21604,13 @@
     </row>
     <row r="983" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A983" t="s">
-        <v>1920</v>
+        <v>1901</v>
       </c>
       <c r="B983" t="s">
-        <v>1920</v>
+        <v>1901</v>
       </c>
       <c r="D983">
-        <v>1082</v>
+        <v>1063</v>
       </c>
       <c r="G983" t="s">
         <v>1877</v>
@@ -21507,13 +21618,13 @@
     </row>
     <row r="984" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A984" t="s">
-        <v>1921</v>
+        <v>1902</v>
       </c>
       <c r="B984" t="s">
-        <v>1921</v>
+        <v>1902</v>
       </c>
       <c r="D984">
-        <v>1083</v>
+        <v>1064</v>
       </c>
       <c r="G984" t="s">
         <v>1877</v>
@@ -21521,13 +21632,13 @@
     </row>
     <row r="985" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A985" t="s">
-        <v>1922</v>
+        <v>1903</v>
       </c>
       <c r="B985" t="s">
-        <v>1922</v>
+        <v>1903</v>
       </c>
       <c r="D985">
-        <v>1084</v>
+        <v>1065</v>
       </c>
       <c r="G985" t="s">
         <v>1877</v>
@@ -21535,13 +21646,13 @@
     </row>
     <row r="986" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A986" t="s">
-        <v>1923</v>
+        <v>1904</v>
       </c>
       <c r="B986" t="s">
-        <v>1923</v>
+        <v>1904</v>
       </c>
       <c r="D986">
-        <v>1085</v>
+        <v>1066</v>
       </c>
       <c r="G986" t="s">
         <v>1877</v>
@@ -21549,13 +21660,13 @@
     </row>
     <row r="987" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A987" t="s">
-        <v>1924</v>
+        <v>1905</v>
       </c>
       <c r="B987" t="s">
-        <v>1924</v>
+        <v>1905</v>
       </c>
       <c r="D987">
-        <v>1086</v>
+        <v>1067</v>
       </c>
       <c r="G987" t="s">
         <v>1877</v>
@@ -21563,13 +21674,13 @@
     </row>
     <row r="988" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A988" t="s">
-        <v>1925</v>
+        <v>1906</v>
       </c>
       <c r="B988" t="s">
-        <v>1925</v>
+        <v>1906</v>
       </c>
       <c r="D988">
-        <v>1087</v>
+        <v>1068</v>
       </c>
       <c r="G988" t="s">
         <v>1877</v>
@@ -21577,13 +21688,13 @@
     </row>
     <row r="989" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A989" t="s">
-        <v>1926</v>
+        <v>1907</v>
       </c>
       <c r="B989" t="s">
-        <v>1926</v>
+        <v>1907</v>
       </c>
       <c r="D989">
-        <v>1088</v>
+        <v>1069</v>
       </c>
       <c r="G989" t="s">
         <v>1877</v>
@@ -21591,13 +21702,13 @@
     </row>
     <row r="990" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A990" t="s">
-        <v>1927</v>
+        <v>1908</v>
       </c>
       <c r="B990" t="s">
-        <v>1927</v>
+        <v>1908</v>
       </c>
       <c r="D990">
-        <v>1089</v>
+        <v>1070</v>
       </c>
       <c r="G990" t="s">
         <v>1877</v>
@@ -21605,13 +21716,13 @@
     </row>
     <row r="991" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A991" t="s">
-        <v>1928</v>
+        <v>1909</v>
       </c>
       <c r="B991" t="s">
-        <v>1928</v>
+        <v>1909</v>
       </c>
       <c r="D991">
-        <v>1090</v>
+        <v>1071</v>
       </c>
       <c r="G991" t="s">
         <v>1877</v>
@@ -21619,13 +21730,13 @@
     </row>
     <row r="992" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A992" t="s">
-        <v>1929</v>
+        <v>1910</v>
       </c>
       <c r="B992" t="s">
-        <v>1929</v>
+        <v>1910</v>
       </c>
       <c r="D992">
-        <v>1091</v>
+        <v>1072</v>
       </c>
       <c r="G992" t="s">
         <v>1877</v>
@@ -21633,13 +21744,13 @@
     </row>
     <row r="993" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A993" t="s">
-        <v>1930</v>
+        <v>1911</v>
       </c>
       <c r="B993" t="s">
-        <v>1930</v>
+        <v>1911</v>
       </c>
       <c r="D993">
-        <v>1092</v>
+        <v>1073</v>
       </c>
       <c r="G993" t="s">
         <v>1877</v>
@@ -21647,13 +21758,13 @@
     </row>
     <row r="994" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A994" t="s">
-        <v>1931</v>
+        <v>1912</v>
       </c>
       <c r="B994" t="s">
-        <v>1931</v>
+        <v>1912</v>
       </c>
       <c r="D994">
-        <v>1093</v>
+        <v>1074</v>
       </c>
       <c r="G994" t="s">
         <v>1877</v>
@@ -21661,13 +21772,13 @@
     </row>
     <row r="995" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A995" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="B995" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="D995">
-        <v>1094</v>
+        <v>1075</v>
       </c>
       <c r="G995" t="s">
         <v>1877</v>
@@ -21675,13 +21786,13 @@
     </row>
     <row r="996" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A996" t="s">
-        <v>1933</v>
+        <v>1914</v>
       </c>
       <c r="B996" t="s">
-        <v>1933</v>
+        <v>1914</v>
       </c>
       <c r="D996">
-        <v>1095</v>
+        <v>1076</v>
       </c>
       <c r="G996" t="s">
         <v>1877</v>
@@ -21689,13 +21800,13 @@
     </row>
     <row r="997" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A997" t="s">
-        <v>1934</v>
+        <v>1915</v>
       </c>
       <c r="B997" t="s">
-        <v>1934</v>
+        <v>1915</v>
       </c>
       <c r="D997">
-        <v>1096</v>
+        <v>1077</v>
       </c>
       <c r="G997" t="s">
         <v>1877</v>
@@ -21703,13 +21814,13 @@
     </row>
     <row r="998" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A998" t="s">
-        <v>1935</v>
+        <v>1916</v>
       </c>
       <c r="B998" t="s">
-        <v>1935</v>
+        <v>1916</v>
       </c>
       <c r="D998">
-        <v>1097</v>
+        <v>1078</v>
       </c>
       <c r="G998" t="s">
         <v>1877</v>
@@ -21717,13 +21828,13 @@
     </row>
     <row r="999" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A999" t="s">
-        <v>1936</v>
+        <v>1917</v>
       </c>
       <c r="B999" t="s">
-        <v>1936</v>
+        <v>1917</v>
       </c>
       <c r="D999">
-        <v>1098</v>
+        <v>1079</v>
       </c>
       <c r="G999" t="s">
         <v>1877</v>
@@ -21731,13 +21842,13 @@
     </row>
     <row r="1000" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1000" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="B1000" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="D1000">
-        <v>1099</v>
+        <v>1080</v>
       </c>
       <c r="G1000" t="s">
         <v>1877</v>
@@ -21745,13 +21856,13 @@
     </row>
     <row r="1001" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1001" t="s">
-        <v>1855</v>
+        <v>1919</v>
       </c>
       <c r="B1001" t="s">
-        <v>1855</v>
+        <v>1919</v>
       </c>
       <c r="D1001">
-        <v>1100</v>
+        <v>1081</v>
       </c>
       <c r="G1001" t="s">
         <v>1877</v>
@@ -21759,13 +21870,13 @@
     </row>
     <row r="1002" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1002" t="s">
-        <v>1856</v>
+        <v>1920</v>
       </c>
       <c r="B1002" t="s">
-        <v>1856</v>
+        <v>1920</v>
       </c>
       <c r="D1002">
-        <v>1101</v>
+        <v>1082</v>
       </c>
       <c r="G1002" t="s">
         <v>1877</v>
@@ -21773,13 +21884,13 @@
     </row>
     <row r="1003" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1003" t="s">
-        <v>1857</v>
+        <v>1921</v>
       </c>
       <c r="B1003" t="s">
-        <v>1857</v>
+        <v>1921</v>
       </c>
       <c r="D1003">
-        <v>1102</v>
+        <v>1083</v>
       </c>
       <c r="G1003" t="s">
         <v>1877</v>
@@ -21787,13 +21898,13 @@
     </row>
     <row r="1004" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1004" t="s">
-        <v>1858</v>
+        <v>1922</v>
       </c>
       <c r="B1004" t="s">
-        <v>1858</v>
+        <v>1922</v>
       </c>
       <c r="D1004">
-        <v>1103</v>
+        <v>1084</v>
       </c>
       <c r="G1004" t="s">
         <v>1877</v>
@@ -21801,13 +21912,13 @@
     </row>
     <row r="1005" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1005" t="s">
-        <v>1859</v>
+        <v>1923</v>
       </c>
       <c r="B1005" t="s">
-        <v>1859</v>
+        <v>1923</v>
       </c>
       <c r="D1005">
-        <v>1104</v>
+        <v>1085</v>
       </c>
       <c r="G1005" t="s">
         <v>1877</v>
@@ -21815,13 +21926,13 @@
     </row>
     <row r="1006" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1006" t="s">
-        <v>1860</v>
+        <v>1924</v>
       </c>
       <c r="B1006" t="s">
-        <v>1860</v>
+        <v>1924</v>
       </c>
       <c r="D1006">
-        <v>1105</v>
+        <v>1086</v>
       </c>
       <c r="G1006" t="s">
         <v>1877</v>
@@ -21829,13 +21940,13 @@
     </row>
     <row r="1007" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
-        <v>1861</v>
+        <v>1925</v>
       </c>
       <c r="B1007" t="s">
-        <v>1861</v>
+        <v>1925</v>
       </c>
       <c r="D1007">
-        <v>1106</v>
+        <v>1087</v>
       </c>
       <c r="G1007" t="s">
         <v>1877</v>
@@ -21843,13 +21954,13 @@
     </row>
     <row r="1008" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1008" t="s">
-        <v>1862</v>
+        <v>1926</v>
       </c>
       <c r="B1008" t="s">
-        <v>1862</v>
+        <v>1926</v>
       </c>
       <c r="D1008">
-        <v>1107</v>
+        <v>1088</v>
       </c>
       <c r="G1008" t="s">
         <v>1877</v>
@@ -21857,13 +21968,13 @@
     </row>
     <row r="1009" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
-        <v>1863</v>
+        <v>1927</v>
       </c>
       <c r="B1009" t="s">
-        <v>1863</v>
+        <v>1927</v>
       </c>
       <c r="D1009">
-        <v>1108</v>
+        <v>1089</v>
       </c>
       <c r="G1009" t="s">
         <v>1877</v>
@@ -21871,13 +21982,13 @@
     </row>
     <row r="1010" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
-        <v>1864</v>
+        <v>1928</v>
       </c>
       <c r="B1010" t="s">
-        <v>1864</v>
+        <v>1928</v>
       </c>
       <c r="D1010">
-        <v>1109</v>
+        <v>1090</v>
       </c>
       <c r="G1010" t="s">
         <v>1877</v>
@@ -21885,13 +21996,13 @@
     </row>
     <row r="1011" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1011" t="s">
-        <v>1865</v>
+        <v>1929</v>
       </c>
       <c r="B1011" t="s">
-        <v>1865</v>
+        <v>1929</v>
       </c>
       <c r="D1011">
-        <v>1110</v>
+        <v>1091</v>
       </c>
       <c r="G1011" t="s">
         <v>1877</v>
@@ -21899,13 +22010,13 @@
     </row>
     <row r="1012" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1012" t="s">
-        <v>1866</v>
+        <v>1930</v>
       </c>
       <c r="B1012" t="s">
-        <v>1866</v>
+        <v>1930</v>
       </c>
       <c r="D1012">
-        <v>1111</v>
+        <v>1092</v>
       </c>
       <c r="G1012" t="s">
         <v>1877</v>
@@ -21913,13 +22024,13 @@
     </row>
     <row r="1013" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1013" t="s">
-        <v>1867</v>
+        <v>1931</v>
       </c>
       <c r="B1013" t="s">
-        <v>1867</v>
+        <v>1931</v>
       </c>
       <c r="D1013">
-        <v>1112</v>
+        <v>1093</v>
       </c>
       <c r="G1013" t="s">
         <v>1877</v>
@@ -21927,13 +22038,13 @@
     </row>
     <row r="1014" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1014" t="s">
-        <v>1868</v>
+        <v>1932</v>
       </c>
       <c r="B1014" t="s">
-        <v>1868</v>
+        <v>1932</v>
       </c>
       <c r="D1014">
-        <v>1113</v>
+        <v>1094</v>
       </c>
       <c r="G1014" t="s">
         <v>1877</v>
@@ -21941,13 +22052,13 @@
     </row>
     <row r="1015" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1015" t="s">
-        <v>1869</v>
+        <v>1933</v>
       </c>
       <c r="B1015" t="s">
-        <v>1869</v>
+        <v>1933</v>
       </c>
       <c r="D1015">
-        <v>1114</v>
+        <v>1095</v>
       </c>
       <c r="G1015" t="s">
         <v>1877</v>
@@ -21955,13 +22066,13 @@
     </row>
     <row r="1016" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
-        <v>1870</v>
+        <v>1934</v>
       </c>
       <c r="B1016" t="s">
-        <v>1870</v>
+        <v>1934</v>
       </c>
       <c r="D1016">
-        <v>1115</v>
+        <v>1096</v>
       </c>
       <c r="G1016" t="s">
         <v>1877</v>
@@ -21969,13 +22080,13 @@
     </row>
     <row r="1017" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1017" t="s">
-        <v>1871</v>
+        <v>1935</v>
       </c>
       <c r="B1017" t="s">
-        <v>1871</v>
+        <v>1935</v>
       </c>
       <c r="D1017">
-        <v>1116</v>
+        <v>1097</v>
       </c>
       <c r="G1017" t="s">
         <v>1877</v>
@@ -21983,13 +22094,13 @@
     </row>
     <row r="1018" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1018" t="s">
-        <v>1872</v>
+        <v>1936</v>
       </c>
       <c r="B1018" t="s">
-        <v>1872</v>
+        <v>1936</v>
       </c>
       <c r="D1018">
-        <v>1117</v>
+        <v>1098</v>
       </c>
       <c r="G1018" t="s">
         <v>1877</v>
@@ -21997,13 +22108,13 @@
     </row>
     <row r="1019" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1019" t="s">
-        <v>1873</v>
+        <v>1937</v>
       </c>
       <c r="B1019" t="s">
-        <v>1873</v>
+        <v>1937</v>
       </c>
       <c r="D1019">
-        <v>1118</v>
+        <v>1099</v>
       </c>
       <c r="G1019" t="s">
         <v>1877</v>
@@ -22011,13 +22122,13 @@
     </row>
     <row r="1020" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
-        <v>1874</v>
+        <v>1855</v>
       </c>
       <c r="B1020" t="s">
-        <v>1874</v>
+        <v>1855</v>
       </c>
       <c r="D1020">
-        <v>1119</v>
+        <v>1100</v>
       </c>
       <c r="G1020" t="s">
         <v>1877</v>
@@ -22025,526 +22136,792 @@
     </row>
     <row r="1021" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
-        <v>1701</v>
+        <v>1856</v>
       </c>
       <c r="B1021" t="s">
-        <v>1701</v>
+        <v>1856</v>
       </c>
       <c r="D1021">
-        <v>2007</v>
+        <v>1101</v>
+      </c>
+      <c r="G1021" t="s">
+        <v>1877</v>
       </c>
     </row>
     <row r="1022" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1022" t="s">
-        <v>1702</v>
+        <v>1857</v>
       </c>
       <c r="B1022" t="s">
-        <v>1702</v>
+        <v>1857</v>
       </c>
       <c r="D1022">
-        <v>2008</v>
+        <v>1102</v>
+      </c>
+      <c r="G1022" t="s">
+        <v>1877</v>
       </c>
     </row>
     <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1023" t="s">
-        <v>1703</v>
+        <v>1858</v>
       </c>
       <c r="B1023" t="s">
-        <v>1703</v>
+        <v>1858</v>
       </c>
       <c r="D1023">
-        <v>2009</v>
+        <v>1103</v>
+      </c>
+      <c r="G1023" t="s">
+        <v>1877</v>
       </c>
     </row>
     <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1024" t="s">
-        <v>1704</v>
+        <v>1859</v>
       </c>
       <c r="B1024" t="s">
-        <v>1704</v>
+        <v>1859</v>
       </c>
       <c r="D1024">
-        <v>2047</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1104</v>
+      </c>
+      <c r="G1024" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1025" t="s">
-        <v>1938</v>
+        <v>1860</v>
       </c>
       <c r="B1025" t="s">
-        <v>1938</v>
+        <v>1860</v>
       </c>
       <c r="D1025">
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1105</v>
+      </c>
+      <c r="G1025" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1026" t="s">
-        <v>1939</v>
+        <v>1861</v>
       </c>
       <c r="B1026" t="s">
-        <v>1939</v>
+        <v>1861</v>
       </c>
       <c r="D1026">
-        <v>2081</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1106</v>
+      </c>
+      <c r="G1026" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
-        <v>1940</v>
+        <v>1862</v>
       </c>
       <c r="B1027" t="s">
-        <v>1940</v>
+        <v>1862</v>
       </c>
       <c r="D1027">
-        <v>2082</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1107</v>
+      </c>
+      <c r="G1027" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
-        <v>1941</v>
+        <v>1863</v>
       </c>
       <c r="B1028" t="s">
-        <v>1941</v>
+        <v>1863</v>
       </c>
       <c r="D1028">
-        <v>2083</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1108</v>
+      </c>
+      <c r="G1028" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1029" t="s">
-        <v>1942</v>
+        <v>1864</v>
       </c>
       <c r="B1029" t="s">
-        <v>1942</v>
+        <v>1864</v>
       </c>
       <c r="D1029">
-        <v>2084</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1109</v>
+      </c>
+      <c r="G1029" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1030" t="s">
-        <v>1800</v>
+        <v>1865</v>
       </c>
       <c r="B1030" t="s">
-        <v>1800</v>
-      </c>
-      <c r="C1030" t="s">
-        <v>1799</v>
+        <v>1865</v>
       </c>
       <c r="D1030">
-        <v>3001</v>
-      </c>
-      <c r="I1030"/>
-    </row>
-    <row r="1031" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1110</v>
+      </c>
+      <c r="G1030" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1031" t="s">
-        <v>1802</v>
+        <v>1866</v>
       </c>
       <c r="B1031" t="s">
-        <v>1802</v>
-      </c>
-      <c r="C1031" t="s">
-        <v>1801</v>
+        <v>1866</v>
       </c>
       <c r="D1031">
-        <v>3002</v>
-      </c>
-      <c r="I1031"/>
-    </row>
-    <row r="1032" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1111</v>
+      </c>
+      <c r="G1031" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1032" t="s">
-        <v>1804</v>
+        <v>1867</v>
       </c>
       <c r="B1032" t="s">
-        <v>1804</v>
-      </c>
-      <c r="C1032" t="s">
-        <v>1803</v>
+        <v>1867</v>
       </c>
       <c r="D1032">
-        <v>3003</v>
-      </c>
-      <c r="I1032"/>
-    </row>
-    <row r="1033" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1112</v>
+      </c>
+      <c r="G1032" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1033" t="s">
-        <v>1806</v>
+        <v>1868</v>
       </c>
       <c r="B1033" t="s">
-        <v>1806</v>
-      </c>
-      <c r="C1033" t="s">
-        <v>1805</v>
+        <v>1868</v>
       </c>
       <c r="D1033">
-        <v>3004</v>
-      </c>
-      <c r="I1033"/>
-    </row>
-    <row r="1034" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1113</v>
+      </c>
+      <c r="G1033" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
-        <v>1808</v>
+        <v>1869</v>
       </c>
       <c r="B1034" t="s">
-        <v>1808</v>
-      </c>
-      <c r="C1034" t="s">
-        <v>1807</v>
+        <v>1869</v>
       </c>
       <c r="D1034">
-        <v>3005</v>
-      </c>
-      <c r="I1034"/>
-    </row>
-    <row r="1035" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1114</v>
+      </c>
+      <c r="G1034" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
-        <v>1810</v>
+        <v>1870</v>
       </c>
       <c r="B1035" t="s">
-        <v>1810</v>
-      </c>
-      <c r="C1035" t="s">
-        <v>1809</v>
+        <v>1870</v>
       </c>
       <c r="D1035">
-        <v>3006</v>
-      </c>
-      <c r="I1035"/>
-    </row>
-    <row r="1036" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1115</v>
+      </c>
+      <c r="G1035" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1036" t="s">
-        <v>1812</v>
+        <v>1871</v>
       </c>
       <c r="B1036" t="s">
-        <v>1812</v>
-      </c>
-      <c r="C1036" t="s">
-        <v>1811</v>
+        <v>1871</v>
       </c>
       <c r="D1036">
-        <v>3007</v>
-      </c>
-      <c r="I1036"/>
-    </row>
-    <row r="1037" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1116</v>
+      </c>
+      <c r="G1036" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
-        <v>1814</v>
+        <v>1872</v>
       </c>
       <c r="B1037" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C1037" t="s">
-        <v>1813</v>
+        <v>1872</v>
       </c>
       <c r="D1037">
-        <v>3008</v>
-      </c>
-      <c r="I1037"/>
-    </row>
-    <row r="1038" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1117</v>
+      </c>
+      <c r="G1037" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1038" t="s">
-        <v>1816</v>
+        <v>1873</v>
       </c>
       <c r="B1038" t="s">
-        <v>1816</v>
-      </c>
-      <c r="C1038" t="s">
-        <v>1815</v>
+        <v>1873</v>
       </c>
       <c r="D1038">
-        <v>3009</v>
-      </c>
-      <c r="I1038"/>
-    </row>
-    <row r="1039" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1118</v>
+      </c>
+      <c r="G1038" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1039" t="s">
-        <v>1818</v>
+        <v>1874</v>
       </c>
       <c r="B1039" t="s">
-        <v>1818</v>
-      </c>
-      <c r="C1039" t="s">
-        <v>1817</v>
+        <v>1874</v>
       </c>
       <c r="D1039">
-        <v>3010</v>
-      </c>
-      <c r="I1039"/>
-    </row>
-    <row r="1040" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1119</v>
+      </c>
+      <c r="G1039" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1040" t="s">
-        <v>1820</v>
+        <v>1701</v>
       </c>
       <c r="B1040" t="s">
-        <v>1820</v>
-      </c>
-      <c r="C1040" t="s">
-        <v>1819</v>
+        <v>1701</v>
       </c>
       <c r="D1040">
-        <v>3011</v>
-      </c>
-      <c r="I1040"/>
+        <v>2007</v>
+      </c>
     </row>
     <row r="1041" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
-        <v>1822</v>
+        <v>1702</v>
       </c>
       <c r="B1041" t="s">
-        <v>1822</v>
-      </c>
-      <c r="C1041" t="s">
-        <v>1821</v>
+        <v>1702</v>
       </c>
       <c r="D1041">
-        <v>3012</v>
-      </c>
-      <c r="I1041"/>
+        <v>2008</v>
+      </c>
     </row>
     <row r="1042" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1042" t="s">
-        <v>1824</v>
+        <v>1703</v>
       </c>
       <c r="B1042" t="s">
-        <v>1824</v>
-      </c>
-      <c r="C1042" t="s">
-        <v>1823</v>
+        <v>1703</v>
       </c>
       <c r="D1042">
-        <v>3013</v>
-      </c>
-      <c r="I1042"/>
+        <v>2009</v>
+      </c>
     </row>
     <row r="1043" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1043" t="s">
-        <v>1826</v>
+        <v>1704</v>
       </c>
       <c r="B1043" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C1043" t="s">
-        <v>1825</v>
+        <v>1704</v>
       </c>
       <c r="D1043">
-        <v>3014</v>
-      </c>
-      <c r="I1043"/>
+        <v>2047</v>
+      </c>
     </row>
     <row r="1044" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1044" t="s">
-        <v>1828</v>
+        <v>1938</v>
       </c>
       <c r="B1044" t="s">
-        <v>1828</v>
-      </c>
-      <c r="C1044" t="s">
-        <v>1827</v>
+        <v>1938</v>
       </c>
       <c r="D1044">
-        <v>3015</v>
-      </c>
-      <c r="I1044"/>
+        <v>2080</v>
+      </c>
     </row>
     <row r="1045" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1045" t="s">
-        <v>1830</v>
+        <v>1939</v>
       </c>
       <c r="B1045" t="s">
-        <v>1830</v>
-      </c>
-      <c r="C1045" t="s">
-        <v>1829</v>
+        <v>1939</v>
       </c>
       <c r="D1045">
-        <v>3016</v>
-      </c>
-      <c r="I1045"/>
+        <v>2081</v>
+      </c>
     </row>
     <row r="1046" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1046" t="s">
-        <v>1832</v>
+        <v>1940</v>
       </c>
       <c r="B1046" t="s">
-        <v>1832</v>
-      </c>
-      <c r="C1046" t="s">
-        <v>1831</v>
+        <v>1940</v>
       </c>
       <c r="D1046">
-        <v>3017</v>
-      </c>
-      <c r="I1046"/>
+        <v>2082</v>
+      </c>
     </row>
     <row r="1047" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1047" t="s">
-        <v>1834</v>
+        <v>1941</v>
       </c>
       <c r="B1047" t="s">
-        <v>1834</v>
-      </c>
-      <c r="C1047" t="s">
-        <v>1833</v>
+        <v>1941</v>
       </c>
       <c r="D1047">
-        <v>3018</v>
-      </c>
-      <c r="I1047"/>
+        <v>2083</v>
+      </c>
     </row>
     <row r="1048" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1048" t="s">
-        <v>1836</v>
+        <v>1942</v>
       </c>
       <c r="B1048" t="s">
-        <v>1836</v>
-      </c>
-      <c r="C1048" t="s">
-        <v>1835</v>
+        <v>1942</v>
       </c>
       <c r="D1048">
-        <v>3019</v>
-      </c>
-      <c r="I1048"/>
+        <v>2084</v>
+      </c>
     </row>
     <row r="1049" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1049" t="s">
-        <v>1838</v>
+        <v>1800</v>
       </c>
       <c r="B1049" t="s">
-        <v>1838</v>
+        <v>1800</v>
       </c>
       <c r="C1049" t="s">
-        <v>1837</v>
+        <v>1799</v>
       </c>
       <c r="D1049">
-        <v>3020</v>
+        <v>3001</v>
       </c>
       <c r="I1049"/>
     </row>
     <row r="1050" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1050" t="s">
-        <v>1840</v>
+        <v>1802</v>
       </c>
       <c r="B1050" t="s">
-        <v>1840</v>
+        <v>1802</v>
       </c>
       <c r="C1050" t="s">
-        <v>1839</v>
+        <v>1801</v>
       </c>
       <c r="D1050">
-        <v>3021</v>
+        <v>3002</v>
       </c>
       <c r="I1050"/>
     </row>
     <row r="1051" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
-        <v>1842</v>
+        <v>1804</v>
       </c>
       <c r="B1051" t="s">
-        <v>1842</v>
+        <v>1804</v>
       </c>
       <c r="C1051" t="s">
-        <v>1841</v>
+        <v>1803</v>
       </c>
       <c r="D1051">
-        <v>3022</v>
+        <v>3003</v>
       </c>
       <c r="I1051"/>
     </row>
     <row r="1052" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1052" t="s">
-        <v>1844</v>
+        <v>1806</v>
       </c>
       <c r="B1052" t="s">
-        <v>1844</v>
+        <v>1806</v>
       </c>
       <c r="C1052" t="s">
-        <v>1843</v>
+        <v>1805</v>
       </c>
       <c r="D1052">
-        <v>3023</v>
+        <v>3004</v>
       </c>
       <c r="I1052"/>
     </row>
     <row r="1053" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1053" t="s">
-        <v>1846</v>
+        <v>1808</v>
       </c>
       <c r="B1053" t="s">
-        <v>1846</v>
+        <v>1808</v>
       </c>
       <c r="C1053" t="s">
-        <v>1845</v>
+        <v>1807</v>
       </c>
       <c r="D1053">
-        <v>3024</v>
+        <v>3005</v>
       </c>
       <c r="I1053"/>
     </row>
     <row r="1054" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1054" t="s">
-        <v>1848</v>
+        <v>1810</v>
       </c>
       <c r="B1054" t="s">
-        <v>1848</v>
+        <v>1810</v>
       </c>
       <c r="C1054" t="s">
-        <v>1847</v>
+        <v>1809</v>
       </c>
       <c r="D1054">
-        <v>3025</v>
+        <v>3006</v>
       </c>
       <c r="I1054"/>
     </row>
     <row r="1055" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1055" t="s">
-        <v>1850</v>
+        <v>1812</v>
       </c>
       <c r="B1055" t="s">
-        <v>1850</v>
+        <v>1812</v>
       </c>
       <c r="C1055" t="s">
-        <v>1849</v>
+        <v>1811</v>
       </c>
       <c r="D1055">
-        <v>3026</v>
+        <v>3007</v>
       </c>
       <c r="I1055"/>
     </row>
     <row r="1056" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
-        <v>1852</v>
+        <v>1814</v>
       </c>
       <c r="B1056" t="s">
-        <v>1852</v>
+        <v>1814</v>
       </c>
       <c r="C1056" t="s">
-        <v>1851</v>
+        <v>1813</v>
       </c>
       <c r="D1056">
-        <v>3027</v>
+        <v>3008</v>
       </c>
       <c r="I1056"/>
     </row>
     <row r="1057" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1057" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D1057">
+        <v>3009</v>
+      </c>
+      <c r="I1057"/>
+    </row>
+    <row r="1058" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>1817</v>
+      </c>
+      <c r="D1058">
+        <v>3010</v>
+      </c>
+      <c r="I1058"/>
+    </row>
+    <row r="1059" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1059" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D1059">
+        <v>3011</v>
+      </c>
+      <c r="I1059"/>
+    </row>
+    <row r="1060" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1060" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D1060">
+        <v>3012</v>
+      </c>
+      <c r="I1060"/>
+    </row>
+    <row r="1061" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1061" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D1061">
+        <v>3013</v>
+      </c>
+      <c r="I1061"/>
+    </row>
+    <row r="1062" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1062" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>1825</v>
+      </c>
+      <c r="D1062">
+        <v>3014</v>
+      </c>
+      <c r="I1062"/>
+    </row>
+    <row r="1063" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1063" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D1063">
+        <v>3015</v>
+      </c>
+      <c r="I1063"/>
+    </row>
+    <row r="1064" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1064" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D1064">
+        <v>3016</v>
+      </c>
+      <c r="I1064"/>
+    </row>
+    <row r="1065" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1065" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>1831</v>
+      </c>
+      <c r="D1065">
+        <v>3017</v>
+      </c>
+      <c r="I1065"/>
+    </row>
+    <row r="1066" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1066" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D1066">
+        <v>3018</v>
+      </c>
+      <c r="I1066"/>
+    </row>
+    <row r="1067" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1067" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D1067">
+        <v>3019</v>
+      </c>
+      <c r="I1067"/>
+    </row>
+    <row r="1068" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1068" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D1068">
+        <v>3020</v>
+      </c>
+      <c r="I1068"/>
+    </row>
+    <row r="1069" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1069" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D1069">
+        <v>3021</v>
+      </c>
+      <c r="I1069"/>
+    </row>
+    <row r="1070" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1070" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D1070">
+        <v>3022</v>
+      </c>
+      <c r="I1070"/>
+    </row>
+    <row r="1071" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1071" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D1071">
+        <v>3023</v>
+      </c>
+      <c r="I1071"/>
+    </row>
+    <row r="1072" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1072" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D1072">
+        <v>3024</v>
+      </c>
+      <c r="I1072"/>
+    </row>
+    <row r="1073" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1073" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D1073">
+        <v>3025</v>
+      </c>
+      <c r="I1073"/>
+    </row>
+    <row r="1074" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1074" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>1849</v>
+      </c>
+      <c r="D1074">
+        <v>3026</v>
+      </c>
+      <c r="I1074"/>
+    </row>
+    <row r="1075" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1075" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>1851</v>
+      </c>
+      <c r="D1075">
+        <v>3027</v>
+      </c>
+      <c r="I1075"/>
+    </row>
+    <row r="1076" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1076" t="s">
         <v>1854</v>
       </c>
-      <c r="B1057" t="s">
+      <c r="B1076" t="s">
         <v>1854</v>
       </c>
-      <c r="C1057" t="s">
+      <c r="C1076" t="s">
         <v>1853</v>
       </c>
-      <c r="D1057">
+      <c r="D1076">
         <v>3028</v>
       </c>
-      <c r="I1057"/>
+      <c r="I1076"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:J1164">
+    <sortState ref="A2:J1183">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>

</xml_diff>